<commit_message>
Expediente Shannery 2 de mayo de 2025
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B06E951-EF17-4999-8323-679EF68678A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202DF008-26D6-40C6-864B-C550A63B0393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANDREA TOBAR" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="MONICA PARDO" sheetId="8" r:id="rId8"/>
     <sheet name="RUBÉN MARTINEZ" sheetId="9" r:id="rId9"/>
     <sheet name="STEPHANI GUERRERO" sheetId="10" r:id="rId10"/>
+    <sheet name="SHANNERY CHAPARRO" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="345">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -1321,6 +1322,30 @@
 06/03/2025 ASESOR RECIBIÓ CORRECCION Y ESTA EN PROCESO DE REALIZAR LOS AJUSTES NECESARIOS
 28/02/2025 EN TRAMITE DE REVISIÒN Y CORRECCIÒN AUTO ALEGATOS
 21/02/2025 ASESOR INDICA QUE NO HAY NUEVOS ACTOS ADMINISTRATIVOS</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-008134</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE REVOCATORIA DE MANDATO DEL ACTUAL ALCALDE DEL MUNICIPIO DE HONDA TOLIMA, SEÑOR JUAN ENRIQUE RONDON GARCIA</t>
+  </si>
+  <si>
+    <t>TOLIMA</t>
+  </si>
+  <si>
+    <t>HONDA</t>
+  </si>
+  <si>
+    <t>CARLOS HUGO MESA MAYNE</t>
+  </si>
+  <si>
+    <t>REVOCATORIA DE MANDATO</t>
+  </si>
+  <si>
+    <t>02/05/2025 ASIGNADO A LA ASESORA SHANNERY CHAPARRO</t>
+  </si>
+  <si>
+    <t>SHANNERY CHAPARRO</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1496,6 +1521,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1803,7 +1831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2365,6 +2393,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE6D97-3CA4-4CCD-93A2-5E21B1D09E30}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="13">
+        <v>45779</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="13">
+        <v>45779</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="N2" s="6">
+        <v>45779</v>
+      </c>
+      <c r="O2" s="13">
+        <v>45779</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q4"/>

</xml_diff>

<commit_message>
Shannery expediente fecha de caducidad
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202DF008-26D6-40C6-864B-C550A63B0393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B344F3D-AAE9-4529-9DD1-C859D9DA862F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="345">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -2398,7 +2398,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q2"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,7 +2484,9 @@
       <c r="H2" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="J2" s="12" t="s">
         <v>343</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion 6 de mayo 2025
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B344F3D-AAE9-4529-9DD1-C859D9DA862F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06FEEB-8672-4F85-AA51-06BC019181FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANDREA TOBAR" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="351">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -1346,6 +1346,24 @@
   </si>
   <si>
     <t>SHANNERY CHAPARRO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-008157</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE PRÓRROGA PARA LA RECOLECCIÓN DE FIRMAS DE LA CONSULTA POPULAR DE ORIGEN CIUDADANO DENOMINADA "MUNICIPIO DE ALCALÁ EN EL ÁREA METROPOLITANA CENTRO OCCIDENTE AMCO</t>
+  </si>
+  <si>
+    <t>ALCALÁ</t>
+  </si>
+  <si>
+    <t>CARLOS ALCIDES ROJAS PEREZ</t>
+  </si>
+  <si>
+    <t>MECANISMOS DE PARTICIPACIÓN CIUDADANA</t>
+  </si>
+  <si>
+    <t>05/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1525,6 +1543,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2059,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,6 +2409,59 @@
         <v>32</v>
       </c>
     </row>
+    <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45417</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="9">
+        <v>45782</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="N7" s="6">
+        <v>45783</v>
+      </c>
+      <c r="O7" s="6">
+        <v>45714</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2397,7 +2471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE6D97-3CA4-4CCD-93A2-5E21B1D09E30}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualización Anyi 8 de mayo
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06FEEB-8672-4F85-AA51-06BC019181FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BA60AB-FFF9-4C89-ADF6-B318578C6788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANDREA TOBAR" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,25 @@
     <sheet name="STEPHANI GUERRERO" sheetId="10" r:id="rId10"/>
     <sheet name="SHANNERY CHAPARRO" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="345">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -229,40 +242,16 @@
     <t>ORIGEN: JUAN DAVID OSPINA DESTINO: ANDREA TOBAR</t>
   </si>
   <si>
-    <t>CNE-E-DG-2025-004014</t>
-  </si>
-  <si>
     <t>04/03/2025</t>
   </si>
   <si>
-    <t>QUEJA CONTRA EL SEÑOR DANIEL BECERRA MIEMBRO DE LA JUNTA NACIONAL DE COORDINACIÓN DEL MOVIMIENTO POLITICO COLOMBIA HUMANA POR PRESUNTAMENTE UTILIZAR DINEROS DEL PARTIDO SIN DEBIDA AUTORIZACIÓN</t>
-  </si>
-  <si>
     <t>ANONIMO</t>
   </si>
   <si>
-    <t>DELITOS CONTRA LA ADMINISTRACIÓN PUBLICA</t>
-  </si>
-  <si>
-    <t>15/04/2025 OFICIO 006 SE ENVIO AL PETICIONARIO
-15/04/2025 OFICIO 004 SE ENVIO PARA EL MOVIMIENTO POLITICO COLOMBIA HUMANA
-05/03/2025 - RECIBIDO</t>
-  </si>
-  <si>
     <t>PRE-ARCHIVO</t>
   </si>
   <si>
     <t>15/04/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/04/2025 PARA ARCHIVAR EN LA FECHA 29/04/2025
-07/04/2025 OFICIOS DE REVISIÓN DE LAURA
-25/03/2025 OFICIOS PARA REVISIÓN
-14/03/2025 OFICIOS PARA REVISIÓN
-05/03/2025 ENTREGARON REPARTO </t>
-  </si>
-  <si>
-    <t>05/03/2025</t>
   </si>
   <si>
     <t>ANYI AGUIRRE</t>
@@ -2082,7 +2071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2146,7 +2135,7 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -2158,7 +2147,7 @@
         <v>34</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>36</v>
@@ -2173,16 +2162,16 @@
         <v>45729</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
@@ -2191,51 +2180,51 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="I3" s="9">
         <v>46535</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
@@ -2244,7 +2233,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -2252,25 +2241,25 @@
     </row>
     <row r="4" spans="1:17" ht="153" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>24</v>
@@ -2279,25 +2268,25 @@
         <v>46992</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>32</v>
@@ -2305,25 +2294,25 @@
     </row>
     <row r="5" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>24</v>
@@ -2332,7 +2321,7 @@
         <v>46804</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>26</v>
@@ -2341,24 +2330,24 @@
         <v>53</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:17" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>40</v>
@@ -2367,25 +2356,25 @@
         <v>45776</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>26</v>
@@ -2394,7 +2383,7 @@
         <v>45776</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="N6" s="9">
         <v>45776</v>
@@ -2403,7 +2392,7 @@
         <v>45714</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>32</v>
@@ -2411,7 +2400,7 @@
     </row>
     <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>40</v>
@@ -2420,25 +2409,25 @@
         <v>45417</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>26</v>
@@ -2447,7 +2436,7 @@
         <v>45782</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="N7" s="6">
         <v>45783</v>
@@ -2456,7 +2445,7 @@
         <v>45714</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q7" s="7" t="s">
         <v>32</v>
@@ -2535,7 +2524,7 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>40</v>
@@ -2544,25 +2533,25 @@
         <v>45779</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>36</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>26</v>
@@ -2571,7 +2560,7 @@
         <v>45779</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="N2" s="6">
         <v>45779</v>
@@ -2580,7 +2569,7 @@
         <v>45779</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="Q2" s="16" t="s">
         <v>32</v>
@@ -2593,10 +2582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,163 +2646,110 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="C2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="9">
+        <v>46164</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="5">
-        <v>46816</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="Q2" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="I3" s="9">
-        <v>46164</v>
+        <v>46166</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46166</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2889,7 +2825,7 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -2898,10 +2834,10 @@
         <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>36</v>
@@ -2916,7 +2852,7 @@
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
@@ -2925,7 +2861,7 @@
         <v>29</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
@@ -2934,15 +2870,15 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="306" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
@@ -2951,10 +2887,10 @@
         <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>36</v>
@@ -2969,16 +2905,16 @@
         <v>45790</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
@@ -2987,68 +2923,68 @@
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I4" s="9">
         <v>46172</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="408" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>18</v>
@@ -3057,43 +2993,43 @@
         <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I5" s="5">
         <v>46710</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>32</v>
@@ -3101,16 +3037,16 @@
     </row>
     <row r="6" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>36</v>
@@ -3119,25 +3055,25 @@
         <v>36</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I6" s="5">
         <v>46257</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>29</v>
@@ -3146,10 +3082,10 @@
         <v>30</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3225,16 +3161,16 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>36</v>
@@ -3243,60 +3179,60 @@
         <v>36</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I2" s="5">
         <v>45298</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>24</v>
@@ -3305,42 +3241,42 @@
         <v>45701</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>36</v>
@@ -3358,42 +3294,42 @@
         <v>46174</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>36</v>
@@ -3402,25 +3338,25 @@
         <v>36</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I5" s="9">
         <v>46145</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>29</v>
@@ -3429,33 +3365,33 @@
         <v>30</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>24</v>
@@ -3464,33 +3400,33 @@
         <v>46613</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>18</v>
@@ -3499,25 +3435,25 @@
         <v>55</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I7" s="9">
         <v>46783</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>26</v>
@@ -3526,51 +3462,51 @@
         <v>27</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="I8" s="9">
         <v>46342</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>26</v>
@@ -3579,33 +3515,33 @@
         <v>53</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>36</v>
@@ -3614,25 +3550,25 @@
         <v>36</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>29</v>
@@ -3641,7 +3577,7 @@
         <v>29</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>36</v>
@@ -3720,25 +3656,25 @@
     </row>
     <row r="2" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>38</v>
@@ -3747,16 +3683,16 @@
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
@@ -3765,42 +3701,42 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I3" s="9">
         <v>46315</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
@@ -3809,69 +3745,69 @@
         <v>53</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="395.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="I4" s="9">
         <v>46549</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>32</v>
@@ -3879,55 +3815,55 @@
     </row>
     <row r="5" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I5" s="9">
         <v>46636</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4003,52 +3939,52 @@
     </row>
     <row r="2" spans="1:17" ht="344.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I2" s="5">
         <v>45466</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>32</v>
@@ -4056,52 +3992,52 @@
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -4180,16 +4116,16 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>36</v>
@@ -4198,16 +4134,16 @@
         <v>36</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>36</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
@@ -4216,16 +4152,16 @@
         <v>41</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>32</v>
@@ -4233,52 +4169,52 @@
     </row>
     <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I3" s="9">
         <v>46395</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -4357,43 +4293,43 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>37</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I2" s="5">
         <v>44967</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="N2" s="6">
         <v>45776</v>
@@ -4402,7 +4338,7 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>32</v>
@@ -4410,16 +4346,16 @@
     </row>
     <row r="3" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>36</v>
@@ -4428,25 +4364,25 @@
         <v>36</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I3" s="9">
         <v>46232</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="N3" s="6">
         <v>45776</v>
@@ -4455,7 +4391,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -4463,7 +4399,7 @@
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
@@ -4472,7 +4408,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>36</v>
@@ -4490,16 +4426,16 @@
         <v>45790</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="N4" s="6">
         <v>45776</v>
@@ -4508,7 +4444,7 @@
         <v>30</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>32</v>
@@ -4587,7 +4523,7 @@
     </row>
     <row r="2" spans="1:17" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>18</v>
@@ -4596,25 +4532,25 @@
         <v>45700</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="I2" s="13">
         <v>46795</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>26</v>
@@ -4623,7 +4559,7 @@
         <v>45744</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="N2" s="6">
         <v>45777</v>
@@ -4632,7 +4568,7 @@
         <v>45701</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
14 de mayo de 2025
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF60514A-160C-4551-A363-458128D0C8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F3DDB-C9B6-493B-B273-CE680EEF2BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANDREA TOBAR" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="340">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -162,9 +162,6 @@
     <t>27/10/2022</t>
   </si>
   <si>
-    <t>RELACION DE CANDIDATOS QUE NO PRESENTARON INFORME DE INGRESOS Y GASTOS DE CAMPAÑA -CONGRESO ELECCIONES 2022, EN ATENCION A LA OBLIGACION DISPUESTA EN EL ARTICULO 25 DE LA LEY 1475 DE 2011 Y POSIBLE VULNERACION A LOS TERMINOS ESTABLECIDOS EN EL ARTICULO 25 DE LEY 1475 DE 2011 -CONGRESO ELECCIONES 2022. (PARTIDO ALIANZA VERDE)</t>
-  </si>
-  <si>
     <t>VALLE DEL CAUCA</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>CNE-E-DG-2023-012966</t>
   </si>
   <si>
-    <t>09/06/2023</t>
-  </si>
-  <si>
     <t>DENUNCIA POR VIOLACIÓN AL ART. 35 DE LA LEY 1475 DE 2011, POR PARTE DEL PRECANDIDATO AL CONSEJO DE PEREIRA -RISARALDA, VICTOR CARMONA</t>
   </si>
   <si>
@@ -278,34 +272,13 @@
     <t>PUBLICIDAD</t>
   </si>
   <si>
-    <t>12/02/2025 SE ENVIO AUTO CORRE TRASLADO PARA PRESENTAR ALEGATOS A REVISIÓN DE PRIMER FILTRO.
-20/01/2025  RECIBIDO</t>
-  </si>
-  <si>
     <t>12/02/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">29/04/2025 LA PLATAFORMA META DIO RESPUESTA AL AUTO MEJOR PROVEER
-07/04/2025 EN LA FECHA 21/03/2025 SE ENVIA AUTO MEJOR PROVEER PARA FIRMAS
-28/03/2025 EN LA FECHA 21/03/2025 SE ENVIA AUTO MEJOR PROVEER PARA FIRMAS
-13/03/2025 SE ENVIO AUTO MEJOR PROVEER PARA REVISIÓN 
-05/03/2025 EL SEÑOR VICTOR HUGO CARMONA DUQUE ALLEGO ALETOS DE CONCLUSIÓN Y EN LA FECHA 04/03/2025 VENCE TERMINOS PARA ALEGATOS 
-04/03/2025 VENCE TERMINOS PARA ALEGATOS 
-12/02/2025 SE ENVIO AUTO CORRE TRASLADO PARA PRESENTAR ALEGATOS A REVISIÓN DE PRIMER FILTRO.
-EL 17 DE FEBRERO VENCE TERMINOS PARA PRESENTAR DESCARGOS PARA LOS SUJETOS PROCESALES.
-PENDIENTE LAS COMUNICACIONES DE LA RESOLUCIÓN NO. 06680 DEL 18 DE DICIEMBRE DE 2024 DE APERTURA Y FORMULACIÓN DE CARGOS POR PRESUNTA VIOLACIÓN AL ARTICULO 35 DE LA LEY 1475 DE 2011. </t>
-  </si>
-  <si>
-    <t>29/04/2025</t>
-  </si>
-  <si>
     <t>ORIGEN: VANESSA ROSSELL - DESTINO: ANYI AGUIRRE</t>
   </si>
   <si>
     <t>CNE-E-DG-2023-011738</t>
-  </si>
-  <si>
-    <t>24/05/2023</t>
   </si>
   <si>
     <t>DENUNCIA POR VIOLACIÓN AL ART. 35 DE LA LEY 1471 DE 20211, POR PARTE DEL PRE CANDIDATO A LA ALCALDIA DE TULUA -VALLE DEL CAUCA, SANDRA PATRICIA ARRUBLA CARDONA</t>
@@ -320,20 +293,6 @@
     <t>19/03/2025 RECIBIDO POR LA ASESORA ANYI AGUIRRE
 12/02/2025 RESOLUCIÓN No 0597 SE ABRE INVESTIGACION Y SE FORMULAN CARGOS CONTRA LA CIUDADANA SANDRA PATRICIA ARRUBLA POR LA PRESUNTA VULNERACION A LAS NORMAS QUE RIGEN LA PROPAGANDA ELECTORAL
 20/01/2025 - RECIBIDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/04/2025 VENCE TERMINO PARA ALEGATOS
-03/04/2025 SE ENVIA AUTO No 034 PARA FIRMA
-28/03/2025 EN LA FECHA 27 DE MARZO DE 2025 VENCEN TERMINOS PARA PRESENTAR DESCARGOS
-17/03/2025 SIGUE EN ESPERA SE QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO, NO HAN PRESENTADO DESCARGO
-06/03/2025 SIGUE EN ESPERA SE QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
-27/02/2025 EN ESPERA QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
-20/02/2025 EN ESPERA QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
-05/02/2025 SE ENVIO A RADICAR A SALA 
-31/01/2025 LA PROYECCION DEL ACTO ADMINISTRATIVO QUE ABRE INVESTIGACIÓN Y FORMULA CARGOS  ESTA  EN REVISION DE SHAN </t>
-  </si>
-  <si>
-    <t>30/04/2025</t>
   </si>
   <si>
     <t>ORIGEN: VANESSA ROSSELL - JUAN DAVID OSPINA DESTINO: ANYI AGUIRRE</t>
@@ -1136,34 +1095,7 @@
     <t>RUBÉN MARTINEZ</t>
   </si>
   <si>
-    <t>CNE-E-DG-2022-022511 - BOGOTÁ D.C</t>
-  </si>
-  <si>
-    <t>01/04/2025 RESOLUCIÓN No 1472 POR MEDIO DE LA CUAL SE RESUEVE RECURSO DE REPOSICIÓN DEL EX GERENTE
-12/02/2025 RESOLUCIÓN No. 0616 POR MEDIO DE LA CUAL SE RESUELVE RECURSO DE REPOSICIÓN INTERPUESTO POR EL  EXCANDIDATO
-07/11/24 RESOLUCIÓN N° 5873 MEDIANTE LA CUAL SE SANCIONA AL EX CANDIDATO Y SU EX GERENTE APROBADA EN SALA EL 7 DE NOVIEMBRE. TÉRMINO PARA INTERPONER RECURSO HASTA EL 21/01/2025.
-28/08/24 AUTO NO. 116 CORRIGE AUTO 105 Y CORRE TRASLADO DE ALEGATOS DE CONCLUSIÓN. FINALIZA TÉRMINO PARA PRESENTAR ALEGATOS EL 19/09.
-30/07/24 AUTO NO. 105 CORRE TRASLADO PARA PRESENTAR ALEGATOS DE CONCLUSIÓN.
-17/04/24 RESOLUCIÓN NO. 02077 POR MEDIO DE LA CUAL SE APERTURA Y SE FORMULA CARGOS. VENCE TÉRMINO PARA PRESENTAR DESCARGOS EL 25/07/24.
-21/03/24 PONENCIA DE APERTURA RADICADA PARA LA SALA DEL 10/04/24.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/04/2025 PENDIENTE COMUNICACIONES PARA ARCHIVO 
-07/04/2025 PENDIENTE COMUNICACIONES PARA ARCHIVO 
-28/03/2025 ENTRO PARA SALA EL 1 DE ABRIL DE 2025
-13/03/2025 SE RADICÓ EN SALA PONENCIA POR MEDIO DE LA CUAL SE REVUELVE RECURSO DE REPOSICIÓN
-06/03/2025 PONENCIA POR MEDIO DE LA CUAL SE RESUELVE RECURSO DE REPOSICIÓN DEL EXGERENTE DE CAMPAÑA EN SEGUNDO FILTRO.
-27/02/2025 PONENCIA POR MEDIO DE LA CUAL SE RESUELVE RECURSO DE REPOSICIÓN INTERPUESTO POR EL EXGERENTE DE CAMPAÑA EN REVISIÓN DE SEGUNDO FILTRO.
-20/02/2025 PENDIENTE DE RESOLVER RECURSO DE REPOSICIÓN DEL EXGERENTE.
-13/02/2025 PENDIENTE COMUNICACIONES PARA ARCHIVAR
-RADICADA EN SALA EL DÍA 05/02/2025, PONENCIA POR MEDIO DE LA CUAL SE RESUELVE RECURSO DE REPOSICIÓN 
-PONENCIA POR MEDIO DE LA CUAL SE RESUELVE RECURSO DE REPOSICIÓN EN REVISIÓN DE LAURA 28/01/2025 </t>
-  </si>
-  <si>
     <t>STEPHANI GUERRERO</t>
-  </si>
-  <si>
-    <t>ORIGEN: MARGARITA RONCALLO DESTINO: STEPHANI GUERRERO</t>
   </si>
   <si>
     <t>CNE-E-DG-2024-012113</t>
@@ -1365,6 +1297,36 @@
   </si>
   <si>
     <t>12/05/ 2025 RECIBIDO POR EL ASESOR</t>
+  </si>
+  <si>
+    <t>14/04/2025AUTO No 034 -TRASLADO DE ALEGATOS PUBLICIDAD
+20/03/2025 AUTO 028- PRUEBAS PUBLICIDAD MEJOR PROVEER
+12/02/2025 SE ENVIO AUTO CORRE TRASLADO PARA PRESENTAR ALEGATOS A REVISIÓN DE PRIMER FILTRO.
+20/01/2025  RECIBIDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/04/2025SE ENVÍO RESOLUCIÓN QUE DA POR TERMINADO A REVISIÓN DE LAURA
+29/04/2025 LA PLATAFORMA META DIO RESPUESTA AL AUTO MEJOR PROVEER
+07/04/2025 EN LA FECHA 21/03/2025 SE ENVIA AUTO MEJOR PROVEER PARA FIRMAS
+28/03/2025 EN LA FECHA 21/03/2025 SE ENVIA AUTO MEJOR PROVEER PARA FIRMAS
+13/03/2025 SE ENVIO AUTO MEJOR PROVEER PARA REVISIÓN 
+05/03/2025 EL SEÑOR VICTOR HUGO CARMONA DUQUE ALLEGO ALETOS DE CONCLUSIÓN Y EN LA FECHA 04/03/2025 VENCE TERMINOS PARA ALEGATOS 
+04/03/2025 VENCE TERMINOS PARA ALEGATOS 
+12/02/2025 SE ENVIO AUTO CORRE TRASLADO PARA PRESENTAR ALEGATOS A REVISIÓN DE PRIMER FILTRO.
+EL 17 DE FEBRERO VENCE TERMINOS PARA PRESENTAR DESCARGOS PARA LOS SUJETOS PROCESALES.
+PENDIENTE LAS COMUNICACIONES DE LA RESOLUCIÓN NO. 06680 DEL 18 DE DICIEMBRE DE 2024 DE APERTURA Y FORMULACIÓN DE CARGOS POR PRESUNTA VIOLACIÓN AL ARTICULO 35 DE LA LEY 1475 DE 2011. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/05/2025PROYECTANDO RESOLUCIÓN - LA CANDIDATA NO HA ALLEGADO ALEGATOS
+30/04/2025 VENCE TERMINO PARA ALEGATOS
+03/04/2025 SE ENVIA AUTO No 034 PARA FIRMA
+28/03/2025 EN LA FECHA 27 DE MARZO DE 2025 VENCEN TERMINOS PARA PRESENTAR DESCARGOS
+17/03/2025 SIGUE EN ESPERA SE QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO, NO HAN PRESENTADO DESCARGO
+06/03/2025 SIGUE EN ESPERA SE QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
+27/02/2025 EN ESPERA QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
+20/02/2025 EN ESPERA QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
+05/02/2025 SE ENVIO A RADICAR A SALA 
+31/01/2025 LA PROYECCION DEL ACTO ADMINISTRATIVO QUE ABRE INVESTIGACIÓN Y FORMULA CARGOS  ESTA  EN REVISION DE SHAN </t>
   </si>
 </sst>
 </file>
@@ -2000,34 +1962,34 @@
     </row>
     <row r="3" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="H3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
@@ -2036,7 +1998,7 @@
         <v>29</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
@@ -2053,55 +2015,55 @@
     </row>
     <row r="4" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="I4" s="9">
         <v>46779</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2111,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,45 +2137,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="I2" s="9">
+        <v>46535</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="5">
-        <v>45729</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>293</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
@@ -2221,275 +2183,222 @@
       <c r="O2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
+      <c r="P2" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="153" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="H3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="9">
+        <v>46992</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>298</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="I3" s="9">
-        <v>46535</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>303</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="153" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="B4" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>153</v>
+        <v>301</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>307</v>
+        <v>159</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="9">
-        <v>46992</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>310</v>
+        <v>46804</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>305</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>57</v>
+      <c r="L4" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>153</v>
+        <v>307</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>312</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45776</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="F5" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>316</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="9">
-        <v>46804</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>317</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>53</v>
+      <c r="L5" s="9">
+        <v>45776</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>319</v>
+        <v>316</v>
+      </c>
+      <c r="N5" s="9">
+        <v>45776</v>
+      </c>
+      <c r="O5" s="9">
+        <v>45714</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="9">
-        <v>45776</v>
+        <v>45417</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>326</v>
+        <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>327</v>
+        <v>329</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>330</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>195</v>
+        <v>331</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="9">
-        <v>45776</v>
+        <v>45782</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="N6" s="9">
-        <v>45776</v>
-      </c>
-      <c r="O6" s="9">
+        <v>332</v>
+      </c>
+      <c r="N6" s="6">
+        <v>45783</v>
+      </c>
+      <c r="O6" s="6">
         <v>45714</v>
       </c>
-      <c r="P6" s="7" t="s">
-        <v>294</v>
+      <c r="P6" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="9">
-        <v>45417</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="9">
-        <v>45782</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="N7" s="6">
-        <v>45783</v>
-      </c>
-      <c r="O7" s="6">
-        <v>45714</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2566,34 +2475,34 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="13">
         <v>45779</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>26</v>
@@ -2602,7 +2511,7 @@
         <v>45779</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="N2" s="6">
         <v>45779</v>
@@ -2611,7 +2520,7 @@
         <v>45779</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="Q2" s="16" t="s">
         <v>32</v>
@@ -2626,8 +2535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,78 +2599,78 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45086</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="I2" s="9">
         <v>46164</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>69</v>
+      <c r="J2" s="7" t="s">
+        <v>337</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="9">
+        <v>45761</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="N2" s="6">
+        <v>45791</v>
+      </c>
+      <c r="O2" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45070</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>24</v>
@@ -2769,29 +2678,29 @@
       <c r="I3" s="9">
         <v>46166</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>79</v>
+      <c r="J3" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>53</v>
+      <c r="L3" s="9">
+        <v>45735</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>30</v>
+        <v>339</v>
+      </c>
+      <c r="N3" s="6">
+        <v>45761</v>
+      </c>
+      <c r="O3" s="6">
+        <v>45691</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2867,7 +2776,7 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
@@ -2876,25 +2785,25 @@
         <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="I2" s="5">
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
@@ -2903,7 +2812,7 @@
         <v>29</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
@@ -2912,15 +2821,15 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="306" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
@@ -2929,34 +2838,34 @@
         <v>33</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="I3" s="9">
         <v>45790</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
@@ -2965,113 +2874,113 @@
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I4" s="9">
         <v>46172</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="408" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I5" s="5">
         <v>46710</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>32</v>
@@ -3079,43 +2988,43 @@
     </row>
     <row r="6" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I6" s="5">
         <v>46257</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>29</v>
@@ -3124,10 +3033,10 @@
         <v>30</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3139,7 +3048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J8" workbookViewId="0">
+    <sheetView topLeftCell="J8" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:Q10"/>
     </sheetView>
   </sheetViews>
@@ -3203,78 +3112,78 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I2" s="5">
         <v>45298</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>24</v>
@@ -3283,51 +3192,51 @@
         <v>45701</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>24</v>
@@ -3336,69 +3245,69 @@
         <v>46174</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I5" s="9">
         <v>46145</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>29</v>
@@ -3407,33 +3316,33 @@
         <v>30</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>24</v>
@@ -3442,60 +3351,60 @@
         <v>46613</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I7" s="9">
         <v>46783</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>26</v>
@@ -3504,113 +3413,113 @@
         <v>27</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I8" s="9">
         <v>46342</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>29</v>
@@ -3619,42 +3528,42 @@
         <v>29</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="48" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C10" s="19">
         <v>45782</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>26</v>
@@ -3663,7 +3572,7 @@
         <v>45789</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="N10" s="5">
         <v>45789</v>
@@ -3672,10 +3581,10 @@
         <v>45789</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3751,43 +3660,43 @@
     </row>
     <row r="2" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="5">
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>29</v>
@@ -3796,113 +3705,113 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I3" s="9">
         <v>46315</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="395.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I4" s="9">
         <v>46549</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>32</v>
@@ -3910,55 +3819,55 @@
     </row>
     <row r="5" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="I5" s="9">
         <v>46636</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4034,52 +3943,52 @@
     </row>
     <row r="2" spans="1:17" ht="344.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="I2" s="5">
         <v>45466</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>32</v>
@@ -4087,52 +3996,52 @@
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -4211,52 +4120,52 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>32</v>
@@ -4264,52 +4173,52 @@
     </row>
     <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="I3" s="9">
         <v>46395</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -4388,43 +4297,43 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I2" s="5">
         <v>44967</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="N2" s="6">
         <v>45776</v>
@@ -4433,7 +4342,7 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>32</v>
@@ -4441,43 +4350,43 @@
     </row>
     <row r="3" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I3" s="9">
         <v>46232</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="N3" s="6">
         <v>45776</v>
@@ -4486,7 +4395,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>32</v>
@@ -4494,7 +4403,7 @@
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
@@ -4503,34 +4412,34 @@
         <v>33</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="I4" s="9">
         <v>45790</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="N4" s="6">
         <v>45776</v>
@@ -4539,7 +4448,7 @@
         <v>30</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>32</v>
@@ -4618,7 +4527,7 @@
     </row>
     <row r="2" spans="1:17" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>18</v>
@@ -4627,25 +4536,25 @@
         <v>45700</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="I2" s="13">
         <v>46795</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>26</v>
@@ -4654,7 +4563,7 @@
         <v>45744</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="N2" s="6">
         <v>45777</v>
@@ -4663,7 +4572,7 @@
         <v>45701</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
actualizacion 15 de mayo
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322F3DDB-C9B6-493B-B273-CE680EEF2BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21C19DD-71F7-4622-A7E6-0F1A52647703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ANDREA TOBAR" sheetId="1" r:id="rId1"/>
-    <sheet name="ANYI AGUIRRE" sheetId="2" r:id="rId2"/>
-    <sheet name="GENESIS CUELLO" sheetId="3" r:id="rId3"/>
-    <sheet name="JHON TRUJILLO" sheetId="4" r:id="rId4"/>
-    <sheet name="JULIANA NUÑEZ" sheetId="5" r:id="rId5"/>
-    <sheet name="LAURA ORTEGON" sheetId="6" r:id="rId6"/>
-    <sheet name="MIGUEL CALDERON" sheetId="7" r:id="rId7"/>
-    <sheet name="MONICA PARDO" sheetId="8" r:id="rId8"/>
-    <sheet name="RUBÉN MARTINEZ" sheetId="9" r:id="rId9"/>
-    <sheet name="STEPHANI GUERRERO" sheetId="10" r:id="rId10"/>
-    <sheet name="SHANNERY CHAPARRO" sheetId="11" r:id="rId11"/>
+    <sheet name="ANYI AGUIRRE" sheetId="2" r:id="rId1"/>
+    <sheet name="GENESIS CUELLO" sheetId="3" r:id="rId2"/>
+    <sheet name="JHON TRUJILLO" sheetId="4" r:id="rId3"/>
+    <sheet name="JULIANA NUÑEZ" sheetId="5" r:id="rId4"/>
+    <sheet name="LAURA ORTEGON" sheetId="6" r:id="rId5"/>
+    <sheet name="MIGUEL CALDERON" sheetId="7" r:id="rId6"/>
+    <sheet name="MONICA PARDO" sheetId="8" r:id="rId7"/>
+    <sheet name="RUBÉN MARTINEZ" sheetId="9" r:id="rId8"/>
+    <sheet name="STEPHANI GUERRERO" sheetId="10" r:id="rId9"/>
+    <sheet name="SHANNERY CHAPARRO" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="322">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -100,9 +99,6 @@
   </si>
   <si>
     <t>LORDUY</t>
-  </si>
-  <si>
-    <t>12/12/2024</t>
   </si>
   <si>
     <t>PRESUNTA VULNERACIÓN DEL ART. 23 DE LA LEY 1475 DE 2011, LIMITES A LA FINANCIACIÓN PRIVADA</t>
@@ -133,27 +129,10 @@
     <t>01/04/2025</t>
   </si>
   <si>
-    <t>28/04/2025 EN ESPERA DE COMUNICACIONES PARA INICIAR AUTO DE ALEGATOS
-07/04/2025 EN ESPERA DE SU DEBIDA NOTIFICACION
-27/03/2025 SE REALIZA FORMULACIÓN DE CARGOS EN CONTRA DEL EXCANDIDATO, SE RADICO EN SALA EL 20 DE MARZO 
-14/03/2025 EN PROCESO DE REALIZACION RESOLUCION DE FORMULACION DE CARGOS AL EX GERENTE DE CAMPAÑA 
-06/03/2025 EN ESPERA DE TERMINO PARA REALIZAR AUTO DE ALEGATOS (10/03/2025)
-27/02/2025 - EN ESPERA DEL TERMINO PARA INICIAR AUTO DE ALEGATOS DE CONCLUSIÓN. 
-21/02/2025 - EN ESPERA DE QUE ALLEGUEN DESCARGOS
-13/02/2024 - EN ESPERA DE COMUNICACIONES 
-04/02/2025 A LA ESPERA DE COMUNICACIONES
-23/01/2025 EN ESPERA DE COMUNICACIÓN
-15/01/2025 PONENCIA PARA RADICAR EN SALA 
-PENDIENTE EN NOTIFICACION</t>
-  </si>
-  <si>
     <t>28/04/2025</t>
   </si>
   <si>
     <t>03/02/2025</t>
-  </si>
-  <si>
-    <t>ANDREA TOBAR</t>
   </si>
   <si>
     <t>NO</t>
@@ -196,13 +175,7 @@
 11/04/2025 RECIBIDO</t>
   </si>
   <si>
-    <t>28/04/2025 A LA ESPERA DE COMUNICACIONES</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2025-001116</t>
-  </si>
-  <si>
-    <t>27/01/2025</t>
   </si>
   <si>
     <t>CONFORMACIÓN DEL DIRECTORIO DEPARTAMENTAL DEL VALLE DE CAUCA DEL PARTIDO DE LA UNION POR LA GENTE - PARTIDO DE LA U</t>
@@ -223,22 +196,9 @@
     <t>19/03/2025</t>
   </si>
   <si>
-    <t>28/04/2025 SE REALIZA NUEVO AUTO QUE EXHORTA EN REVISIÓN DE SHANNERY
-21/04/2025 EL REPRESENTANTE LEGAL ALLEGA PARCIALMENTE LO SOLICITADO POR AUTO 032
-07/04/2025 SE REALIZO AUTO 032 DEL 2 DE ABRIL QUE EXHORTA AL PARTIDO - SE ENVIA PARA SU DEBIDA FIRMA POR PARTE DEL PRESIDENTE EL 2 DE ABRIL DE 2025 
-27/03/2025 REALIZACIÓN DE AUTO DE INSTAR
-17/03/2025 UNA VEZ ENVIEN LA INFORMACION SE PROCEDE A INSCRIBIR LOS CANDIDATOS O A NEGAR LA INSCRIPCIÓN
-06/03/2025 SIGUE EN REVISIÓN AUTO
-27/02/2025 AUTO ENVIADO A SHAN EL 25 DE FEBRERO
-20/02/2025 ESTA EN REVISIÓN OTRO AUTO QUE DECRETA PRUEBAS SOLICITANDOLE AL PARTIDO DE LA U DOCUMENTOS PARA LA INSCRIPCIÓN DE DIRECTIVOS DEL DIRECTORIO DEPARTAMENTAL DEL VALLE DEL CAUCA</t>
-  </si>
-  <si>
     <t>31/01/2025</t>
   </si>
   <si>
-    <t>ORIGEN: JUAN DAVID OSPINA DESTINO: ANDREA TOBAR</t>
-  </si>
-  <si>
     <t>04/03/2025</t>
   </si>
   <si>
@@ -248,9 +208,6 @@
     <t>PRE-ARCHIVO</t>
   </si>
   <si>
-    <t>15/04/2025</t>
-  </si>
-  <si>
     <t>ANYI AGUIRRE</t>
   </si>
   <si>
@@ -270,9 +227,6 @@
   </si>
   <si>
     <t>PUBLICIDAD</t>
-  </si>
-  <si>
-    <t>12/02/2025</t>
   </si>
   <si>
     <t>ORIGEN: VANESSA ROSSELL - DESTINO: ANYI AGUIRRE</t>
@@ -370,9 +324,6 @@
     <t>CNE-E-DG-2023-013843 - CNE-E-DG-2023-013856</t>
   </si>
   <si>
-    <t>23/06/2023</t>
-  </si>
-  <si>
     <t>QUEJA POR PUBLICIDAD POLITICA EXTEMPORANEA CONTRA CESAR EMILIO CURA VERGARA ''MILLO'' CANDIDATO A LA ALCALDIA MUNICIPAL DE MONTELIBANO -CORDOBA</t>
   </si>
   <si>
@@ -392,23 +343,6 @@
     <t>20/02/2025</t>
   </si>
   <si>
-    <t>23/04/2025 REVISIÓN PONENCIA DA POR TERMINADO, EN REVISIÓN MONICA PARDO
-07/04/2025 EN OBSERVACION, PROYECTANDO PONENCIA
-31/03/2025 AUN CONTINUA EN PROCESO DE ESTUDIAR EL CASO ACUERDO A LOS ELEMENTOS PROBATORIOS ANEXADOS AL EXPEDIENTE PARA PROYECTAR PONENCIA YA SEA DE SANCIÓN O ACCIÓN
-14/03/2025 SE PROCEDERA A ESTUDIAR EL CASO ACUERDO A LOS ELEMENTOS PROBATORIOS ANEXADOS AL EXPEDIENTE PARA PROYECTAR PONENCIA YA SEA DE SANCIÓN O ACCIÓN
-06/03/2025 SIGUE EN COMUNICACIONES DEL AUTO 018 DE 2025 
-17/02/2025 - RECIBÍ COMUNICACIONES DEL AUTO 018 DE 2025
-12/02/2025 ENVIADO A MAGISTRADO AUTO TRASLADO PARA FIRMA
-29/01/2025 ENVIADO AUTO ALEGATOS PARA REVISIÓN DE SHANNERY
-23/01/2025 SE ENVIA A CORRECCIÓN DE LAURA, AUTO CORRE TRASLADO Y DECRETAN PRUEBAS</t>
-  </si>
-  <si>
-    <t>23/04/2025</t>
-  </si>
-  <si>
-    <t>ORIGEN: VANESSA ROSSELL - DESTINO: GENESIS CUELLO</t>
-  </si>
-  <si>
     <t>06/12/2023</t>
   </si>
   <si>
@@ -446,32 +380,12 @@
 28/02/2025 RECIBIDO</t>
   </si>
   <si>
-    <t>06/03/2025</t>
-  </si>
-  <si>
-    <t>22/04/2025 SE REENVÍA AUTO DE ALEGATOS A MONICA PARDO
-07/04/2025 SE PROYECTARA AUTO ALEGATOS
-31/03/2025 RECIBI COMUNICACIONES EL 26 DE MARZO
-14/03/2025 LA PONENCIA 16994 POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS
-06/03/2025 ASESOR CON INFORMACIÓN AL DÍA
-27/02/2025 - PONENCIA 16994 POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS / ENTRA EN SALA EL 04 DE MARZO DE 2025
-20/02/2025 PONENCIA POR MEDIO DEL CUAL SE FORMULAN CARGOS, EN REVISIÓN DE SHANNERY
-13/02/2025 CORRIGIENDO PONENCIA POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS ARTICULO 34 DE LA LEY 1475 
-06/02/2025 ENVIADA PONENCIA POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS ARTICULO 34 DE LA LEY 1475 A LAURA</t>
-  </si>
-  <si>
     <t>22/04/2025</t>
   </si>
   <si>
-    <t>28/01/2025</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2023-021293</t>
   </si>
   <si>
-    <t>23/08/2023</t>
-  </si>
-  <si>
     <t>PUBLICIDAD PROPAGANDA ELECTORAL</t>
   </si>
   <si>
@@ -479,17 +393,11 @@
   </si>
   <si>
     <t>19/03/2025 RECIBIDO POR LA ASESORA GENESIS CUELLO</t>
-  </si>
-  <si>
-    <t>19/03/2024</t>
   </si>
   <si>
     <t>28/04/2024 PROYECTANDO RECURSO INTERPUESTO A LA RESOLUCIÓN SANCIÓN
 07/04/2025 EN ESTUDIO DE EXPEDIENTE
 31/03/2025 ASESOR INDICA QUE EL EXPEDIENTE ESTA EN REVISIÓN</t>
-  </si>
-  <si>
-    <t>ORIGEN: JUAN DAVID OSPINA DESTINO: GENESIS CUELLO</t>
   </si>
   <si>
     <t>2021-000146 - 2021-000147</t>
@@ -780,9 +688,6 @@
     <t>CNE-E-DG-2023-067381</t>
   </si>
   <si>
-    <t>04/12/2023</t>
-  </si>
-  <si>
     <t>ENCUESTAS ELECTORALES</t>
   </si>
   <si>
@@ -798,18 +703,7 @@
     <t>19/03/2025 RECIBIDO POR LA ASESORA JULIANA NUÑEZ</t>
   </si>
   <si>
-    <t>24/04/2025 ENVIADO A REVISIÓN PONENCIA POR MEDIO DEL CUAL SE SANCIONA A LA FIRMA ENCUESTADORA EXPERTISE SAS
-07/04/2025 ASESOR INDICA QUE EL EXPEDIENTE SE ENCUENTRA EN REVISIÓN
-01/04/2025 - ASESOR INDICA QUE EL EXPEDIENTE SE ENCUENTRA EN REVISIÓN</t>
-  </si>
-  <si>
-    <t>ORIGEN: JUAN DAVID DESTINO: JULIANA NUÑEZ</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2024-023516</t>
-  </si>
-  <si>
-    <t>27/12/2024</t>
   </si>
   <si>
     <t>PRESUNTA ADULTERACIÓN DEL ARTÍCULO 16 DE LA RESOLUCIÓN NO. 4737 DE 2023, A LA ALCALDÍA DE QUIPAMA - BOYACÁ, COALICIÓN "QUIPAMA LA FUERZA QUE NOS UNE", ELECCIONES REALIZADAS EL 29 DE OCTUBRE DEL 2023</t>
@@ -830,28 +724,7 @@
  PENDIENTE DECISIÓN DEL MAGISTRADO CÉSAR LORDUY</t>
   </si>
   <si>
-    <t>24/02/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/04/2025 SE ALLEGARON LAS DECLARACIONES EXTRA JUICIO REMITIDAS POR EL SEÑOR FELIX ALEJANDRO GUTIERREZ VEGA
-26/02/2025 RECIBIDAS LAS COMUNICACIONES DEL AUTO 022
-07/04/2025 SIGUEN PENDIENTES LAS COMUNICACIONES DEL AUTO 022
-1/04/2025 SIGUEN PENDIENTES LAS COMUNICACIONES DEL AUTO 022
-17/03/2025 SIGUE EN COMUNICACIOES DEL AUTO 022 DEL 24 DE FEBRERO DE 2025 
-06/03/2025 EN COMUNICACIOES DEL AUTO 022 DEL 24 DE FEBRERO DE 2025 
-25/02/2025 SE COMUNICÓ EL AUTO 022 DEL 24 DE FEBRERO DE 2025 
-20/02/2025 SE PROFIRIO EL AUTO 017 Y SE NOFITICÓ EL DÍA 17/02/2025
-06/02/2025 - A LA ESPERA DECISIÓN DEL PARTIDO CAMBIO RADICAL 
-A LA ESPERA DECISIÓN DEL PARTIDO CAMBIO RADICAL </t>
-  </si>
-  <si>
-    <t>04/04/2025</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2024-017268</t>
-  </si>
-  <si>
-    <t>06/09/2024</t>
   </si>
   <si>
     <t>DENUNCIA POR VIOLENCIA PÓLITICA HACIA LA MUJER EN EL CONCEJO MUNICIPAL DE ZIPAQUIRÁ - CUNDINAMARCA</t>
@@ -871,22 +744,7 @@
 20-01-2025 - RECIBIDO</t>
   </si>
   <si>
-    <t xml:space="preserve">15/04/2025 ENVIADA PONENCIA POR MEDIO DEL CUAL SE DA POR TERMINADO AL PARTIDO ALIANZA VERDE, EN REVISIÓN POR MIGUEL
-01/04/2025 OFICIO 050 AUN EN TRÁMITE DE COMUNICACIONES
-17/03/2025 SIGUE EN COMUNICACIONES DEL OFICIO 050
-06/03/2025 EN COMUNICACIONES DEL OFICIO 050 EL DIA 19/02/2025
-SE COMUNICÓ EL OFICIO 050 EL DIA 19/02/2025
-17/02/2025 SE NOTIFICO EL AUTO 010 DEL 23 DE ENERO DEL 2025 
-24/01/2025 SE NOTIFICO EL AUTO 010 DEL 23 DE ENERO DEL 2025 </t>
-  </si>
-  <si>
-    <t>ORIGEN: VANESSA ROSSELL - DESTINO: JULIANA NUÑEZ</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2023-014262 - CNE-E-DG-2023-014265</t>
-  </si>
-  <si>
-    <t>23/06/2024</t>
   </si>
   <si>
     <t>SOLICITUD DE RECONOCIMIENTO DEL LEGADO DE LA GUAJIRA DEL MOVIMIENTO COLOMBIA HUMANA</t>
@@ -905,9 +763,6 @@
 29/08/2024: AUTO NO 109 DEL 13-08/2024 PRUEBAS DE IMPUGNACIÓN.
 01/02/2024  SE PROFIRIO AUTO NO 006 REITERANDO DECRETO DE PRUEBAS; 
 SE RECIBIERON HASTA EL 25 DE ABRIL DEL AÑO EN CURSO SOPORTES DE COMUNICACIÓN. SE PROFIRIÓ. AUTO N 109 DEL 13 DE AGOSTO DE 2024, EL CUAL DECRETÓ LA PRÁCTICA DE UNAS PRUEBAS PARA MEJOR PROVEER. SE NOTIFICÓ EL 28 DE AGOSTO DE 2024. SE PROFIRIÓ ACTO ADMINISTRATIVO NO 127 DEL 23 DE OCTUBRE DE 2024, A TRAVÉS DEL CUAL SE INSTA AL MOVIMIENTO COLOMBIA HUMANA A DAR CUMPLIMIENTO A LO CONMINADO EN EL ARTÍCULO PRIMERO DEL AUTO 109.</t>
-  </si>
-  <si>
-    <t>16/01/2025</t>
   </si>
   <si>
     <t>08/04/2025 PENDIENTE RESOLUCIÓN PARA SER FIRMADA Y PENDIENTE DE NOTIFICACIONES
@@ -918,16 +773,10 @@
 15/01/2025 SE DEBE CORRER TRASLADO</t>
   </si>
   <si>
-    <t>08/04/2025</t>
-  </si>
-  <si>
     <t>LAURA ORTEGON</t>
   </si>
   <si>
     <t>CNE-E-DG-2025-000141</t>
-  </si>
-  <si>
-    <t>08/01/2025</t>
   </si>
   <si>
     <t>SOLICITUD DE REVOCATORIA DE INSCRIPCIÓN DEL CANDIDATO A LA GOBERNACIÓN DE PUTUMAYO, EL SEÑOR JOHN GABRIEL MOLINA ACOSTA, PARA LAS ELECCIONES ATIPICAS DEL 2025</t>
@@ -1023,9 +872,6 @@
     <t>ROZO</t>
   </si>
   <si>
-    <t>17/06/2020</t>
-  </si>
-  <si>
     <t>CANDIDATOS QUE PRESUNTAMENTE INCUMPLIERON CON LA OBLIGACIÓN DE PRESENTAR SU INFORME DE INGRESOS Y GASTOS DE CAMPAÑA, ELECCIONES 27 DE OCTUBRE DE 2019, PARTIDO CONSERVADOR COLOMBIANO</t>
   </si>
   <si>
@@ -1042,9 +888,6 @@
 RESOLUCION 6283 DEL 9 DE AGOSTO POR LA CUAL SE RESUELVEN UNOS RECURSOS DE REPOSICION</t>
   </si>
   <si>
-    <t>19/11/2024</t>
-  </si>
-  <si>
     <t>MONICA PARDO</t>
   </si>
   <si>
@@ -1056,9 +899,6 @@
   <si>
     <t>05/02/2025 AUTO DELEGATOS DE CONCLUSION
 28/02/2024 RES. 1501 SE ABRE INVESTIGACION Y FORMULA CARGOS</t>
-  </si>
-  <si>
-    <t>05/02/2025</t>
   </si>
   <si>
     <t>CNE-E-DG-2022-023717</t>
@@ -1099,9 +939,6 @@
   </si>
   <si>
     <t>CNE-E-DG-2024-012113</t>
-  </si>
-  <si>
-    <t>28/05/2024</t>
   </si>
   <si>
     <t>ACCIÓN DE PROTECCION DE DERECHOS DE OPOSICIÓN CONTRA ALCALDIA DE ACHÍ- BOLIVAR POR POSIBLE VULNERCIÓN AL ARTICULO 16 DE LA LEY 1909 DE 2018</t>
@@ -1152,21 +989,7 @@
     <t>CAMILO MORENO</t>
   </si>
   <si>
-    <t>04/03/2025 AUTO No 025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO Y SE DECRETAN PRUEBAS
-27/02/2025 RECIBIDO</t>
-  </si>
-  <si>
-    <t>28/04/2025 EN REVISIÓN DE SHANNERY AUTO DECRETA PRUEBA
-07/04/2025 EN ESPERA DE LOS TERMINOS PARA QUE SE ALLEGUEN PRUEBAS
-28/03/2025 EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS
-14/03/2025  EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS
-06/03/2025 EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2025-003216</t>
-  </si>
-  <si>
-    <t>21/02/2025</t>
   </si>
   <si>
     <t xml:space="preserve">QUEJA SOBRE LA FINANCIACIÓN DE LA CAMPAÑA COMO CANDIDATO, DEL ACTUAL ALCALDE DEL MUNICIPIO DE COTA - CUNDINAMARCA, SEÑOR NESTOR ORLANDO BALSERO GARCÍA </t>
@@ -1182,42 +1005,9 @@
 19/03/2025 RECIBIDO POR LA ASESORA STEPHANI GUERRERO</t>
   </si>
   <si>
-    <t>15/04/2025 EN ESPERA DE LOS TERMINOS PARA QUE SE ALLEGUEN PRUEBAS
-07/04/2025 PENDIENTE DE COMUNICACIONES
-28/03/2025 AUTO AVOCA EN REVISIÓN DE PRIMER FILTRO EL 20 DE MARZO DE 2025
-17/03/2025 EN PROYECCIÓN AUTO QUE AVOCA
-06/03/2025 ASESOR INDICA QUE EL EXPEDIENTE SIGUE EN REVISIÓN</t>
-  </si>
-  <si>
-    <t>25/02/2025</t>
-  </si>
-  <si>
     <t>ORIGEN: JUAN DAVID OSPINA DESTINO: STEPHANI GUERRERO</t>
   </si>
   <si>
-    <t>29/04/2025 AUN ESTA EN TRÁMITE DE ARCHIVO
-07/04/2025 AUN ESTA EN TRÁMITE DE ARCHIVO
-31/03/2025 AUN ESTA EN TRÁMITE DE ARCHIVO
-18/03/2025 SIGUE PENDIENTE PARA ARCHIVAR
-27/02/2025 - VERIFICAR LAS COMUNICACIONES PARA ARCHIVAR EXPEDIENTE
-21/02/2025 VERIFICAR LAS COMUNICACIONES PARA ARCHIVAR EXPEDIENTE
-VERIFICAR LAS COMUNICACIONES PARA ARCHIVAR EXPEDIENTE</t>
-  </si>
-  <si>
-    <t>29/04/2025 EN ESPERA DE PROYECCION DE TERMINACION (ALEGATOS RECIBIDOS)
-07/04/2025 EN ESPERA DE PROYECCION DE TERMINACION (ALEGATOS RECIBIDOS)
-31/03/2025 EN ESPERA DE PROYECCION DE TERMINACION (ALEGATOS RECIBIDOS)
-18/03/2025 PENDIENTE PROYECTAR DE TERMINACIÓN (YA SE RECIBIERON LOS ALEGATOS)
-27/02/2025 - NO APLICA SEGUIMIENTO - SIN NOVEDAD EN EXPEDIENTE</t>
-  </si>
-  <si>
-    <t>29/04/2025 EN TRÁMITE DE RECURSOS
-07/04/2025 EN TRÁMITE DE RECURSOS
-31/03/2025 EN TRÁMITE DE RECURSOS
-18/03/2025 PENDIENTE DE RECURSOS
-27/02/2025 - NO APLICA SEGUIMIENTO - SIN NOVEDAD EN EXPEDIENTE</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2025-007754</t>
   </si>
   <si>
@@ -1228,9 +1018,6 @@
   </si>
   <si>
     <t>GUSTAVO GARCIA FIGUEROA Y JENNY LILIANA PULIDO VELASQUEZ</t>
-  </si>
-  <si>
-    <t>29/04/2025 RECIBIDO POR LA ASESORA STPHANI GUERRERO</t>
   </si>
   <si>
     <t>CNE-E-DG-2025-002441</t>
@@ -1282,9 +1069,6 @@
   </si>
   <si>
     <t>MECANISMOS DE PARTICIPACIÓN CIUDADANA</t>
-  </si>
-  <si>
-    <t>05/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
   </si>
   <si>
     <t>CNE-E-DG-2025-008553</t>
@@ -1327,6 +1111,181 @@
 20/02/2025 EN ESPERA QUE CUMPLA EL TERMINO PARA LA PRESENTACIÓN DE DESCARGO
 05/02/2025 SE ENVIO A RADICAR A SALA 
 31/01/2025 LA PROYECCION DEL ACTO ADMINISTRATIVO QUE ABRE INVESTIGACIÓN Y FORMULA CARGOS  ESTA  EN REVISION DE SHAN </t>
+  </si>
+  <si>
+    <t>07/05/2025 AUTO No. 043 DE 2025, POR MEDIO DEL CUAL SE DECRETA LA PRACTICA DE PRUEBAS (PENDIENTE COMUNICACIONES)
+04/03/2025 AUTO No 025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO Y SE DECRETAN PRUEBAS
+27/02/2025 RECIBIDO</t>
+  </si>
+  <si>
+    <t>07/05/2025 AUTO No. 043 DE 2025, POR MEDIO DEL CUAL SE DECRETA LA PRACTICA DE PRUEBAS (PENDIENTE COMUNICACIONES)
+28/04/2025 EN REVISIÓN DE SHANNERY AUTO DECRETA PRUEBA
+07/04/2025 EN ESPERA DE LOS TERMINOS PARA QUE SE ALLEGUEN PRUEBAS
+28/03/2025 EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS
+14/03/2025  EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS
+06/03/2025 EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS</t>
+  </si>
+  <si>
+    <t>14/05/2025 AUTO REITERA EN REVISIÓN DE MIGUEL
+15/04/2025 EN ESPERA DE LOS TERMINOS PARA QUE SE ALLEGUEN PRUEBAS
+07/04/2025 PENDIENTE DE COMUNICACIONES
+28/03/2025 AUTO AVOCA EN REVISIÓN DE PRIMER FILTRO EL 20 DE MARZO DE 2025
+17/03/2025 EN PROYECCIÓN AUTO QUE AVOCA
+06/03/2025 ASESOR INDICA QUE EL EXPEDIENTE SIGUE EN REVISIÓN</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 de 2025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 de 2025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO
+05/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 DE 2025 POR MEDIO DEL CUAL SE AVOCÓ CONOCIMIENTO 
+29/04/2025 RECIBIDO POR LA ASESORA STPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 DE 2025 POR MEDIO DEL CUAL SE AVOCÓ CONOCIMIENTO 
+29/04/2025 RECIBIDO POR LA ASESORA STPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>14/05/2025 AUN ESTA EN TRÁMITE DE ARCHIVO
+07/04/2025 AUN ESTA EN TRÁMITE DE ARCHIVO
+31/03/2025 AUN ESTA EN TRÁMITE DE ARCHIVO
+18/03/2025 SIGUE PENDIENTE PARA ARCHIVAR
+27/02/2025 - VERIFICAR LAS COMUNICACIONES PARA ARCHIVAR EXPEDIENTE
+21/02/2025 VERIFICAR LAS COMUNICACIONES PARA ARCHIVAR EXPEDIENTE
+VERIFICAR LAS COMUNICACIONES PARA ARCHIVAR EXPEDIENTE</t>
+  </si>
+  <si>
+    <t>14/05/2025 EN ESPERA DE PROYECCION DE TERMINACION (ALEGATOS RECIBIDOS)
+07/04/2025 EN ESPERA DE PROYECCION DE TERMINACION (ALEGATOS RECIBIDOS)
+31/03/2025 EN ESPERA DE PROYECCION DE TERMINACION (ALEGATOS RECIBIDOS)
+18/03/2025 PENDIENTE PROYECTAR DE TERMINACIÓN (YA SE RECIBIERON LOS ALEGATOS)
+27/02/2025 - NO APLICA SEGUIMIENTO - SIN NOVEDAD EN EXPEDIENTE</t>
+  </si>
+  <si>
+    <t>14/05/2025 EN TRÁMITE DE RECURSOS
+07/04/2025 EN TRÁMITE DE RECURSOS
+31/03/2025 EN TRÁMITE DE RECURSOS
+18/03/2025 PENDIENTE DE RECURSOS
+27/02/2025 - NO APLICA SEGUIMIENTO - SIN NOVEDAD EN EXPEDIENTE</t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A ANYI AGUIRRE
+22/04/2025 SE REENVÍA AUTO DE ALEGATOS A MONICA PARDO
+07/04/2025 SE PROYECTARA AUTO ALEGATOS
+31/03/2025 RECIBI COMUNICACIONES EL 26 DE MARZO
+14/03/2025 LA PONENCIA 16994 POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS
+06/03/2025 ASESOR CON INFORMACIÓN AL DÍA
+27/02/2025 - PONENCIA 16994 POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS / ENTRA EN SALA EL 04 DE MARZO DE 2025
+20/02/2025 PONENCIA POR MEDIO DEL CUAL SE FORMULAN CARGOS, EN REVISIÓN DE SHANNERY
+13/02/2025 CORRIGIENDO PONENCIA POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS ARTICULO 34 DE LA LEY 1475 
+06/02/2025 ENVIADA PONENCIA POR MEDIO DEL CUAL SE ABRE Y SE FORMULAN CARGOS ARTICULO 34 DE LA LEY 1475 A LAURA</t>
+  </si>
+  <si>
+    <t>ORIGEN: GENESIS CUELLO DESTINO: ANYI AGUIRRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/05/2025 REASIGNADO A LA ASESORA ANYI AGUIRRE
+15/04/2025 ENVIADA PONENCIA POR MEDIO DEL CUAL SE DA POR TERMINADO AL PARTIDO ALIANZA VERDE, EN REVISIÓN POR MIGUEL
+01/04/2025 OFICIO 050 AUN EN TRÁMITE DE COMUNICACIONES
+17/03/2025 SIGUE EN COMUNICACIONES DEL OFICIO 050
+06/03/2025 EN COMUNICACIONES DEL OFICIO 050 EL DIA 19/02/2025
+SE COMUNICÓ EL OFICIO 050 EL DIA 19/02/2025
+17/02/2025 SE NOTIFICO EL AUTO 010 DEL 23 DE ENERO DEL 2025 
+24/01/2025 SE NOTIFICO EL AUTO 010 DEL 23 DE ENERO DEL 2025 </t>
+  </si>
+  <si>
+    <t>ORIGEN: JULIANA NUÑEZ DESTINO: ANYI AGUIRRE</t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A ANYI AGUIRRE
+23/04/2025 REVISIÓN PONENCIA DA POR TERMINADO, EN REVISIÓN MONICA PARDO
+07/04/2025 EN OBSERVACION, PROYECTANDO PONENCIA
+31/03/2025 AUN CONTINUA EN PROCESO DE ESTUDIAR EL CASO ACUERDO A LOS ELEMENTOS PROBATORIOS ANEXADOS AL EXPEDIENTE PARA PROYECTAR PONENCIA YA SEA DE SANCIÓN O ACCIÓN
+14/03/2025 SE PROCEDERA A ESTUDIAR EL CASO ACUERDO A LOS ELEMENTOS PROBATORIOS ANEXADOS AL EXPEDIENTE PARA PROYECTAR PONENCIA YA SEA DE SANCIÓN O ACCIÓN
+06/03/2025 SIGUE EN COMUNICACIONES DEL AUTO 018 DE 2025 
+17/02/2025 - RECIBÍ COMUNICACIONES DEL AUTO 018 DE 2025
+12/02/2025 ENVIADO A MAGISTRADO AUTO TRASLADO PARA FIRMA
+29/01/2025 ENVIADO AUTO ALEGATOS PARA REVISIÓN DE SHANNERY
+23/01/2025 SE ENVIA A CORRECCIÓN DE LAURA, AUTO CORRE TRASLADO Y DECRETAN PRUEBAS</t>
+  </si>
+  <si>
+    <t>ORIGEN:GENESIS CUELLO  DESTINO: ANYI AGUIRRE</t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A LA ASESORA LAURA ORTEGON
+24/04/2025 ENVIADO A REVISIÓN PONENCIA POR MEDIO DEL CUAL SE SANCIONA A LA FIRMA ENCUESTADORA EXPERTISE SAS
+07/04/2025 ASESOR INDICA QUE EL EXPEDIENTE SE ENCUENTRA EN REVISIÓN
+01/04/2025 - ASESOR INDICA QUE EL EXPEDIENTE SE ENCUENTRA EN REVISIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORIGEN: JULIANA NUÑEZ: DESTINO LAURA ORTEGON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/05/2025: REASIGNADO A LA ASESORA LAURA ORTEGON
+04/04/2025 SE ALLEGARON LAS DECLARACIONES EXTRA JUICIO REMITIDAS POR EL SEÑOR FELIX ALEJANDRO GUTIERREZ VEGA
+26/02/2025 RECIBIDAS LAS COMUNICACIONES DEL AUTO 022
+07/04/2025 SIGUEN PENDIENTES LAS COMUNICACIONES DEL AUTO 022
+1/04/2025 SIGUEN PENDIENTES LAS COMUNICACIONES DEL AUTO 022
+17/03/2025 SIGUE EN COMUNICACIOES DEL AUTO 022 DEL 24 DE FEBRERO DE 2025 
+06/03/2025 EN COMUNICACIOES DEL AUTO 022 DEL 24 DE FEBRERO DE 2025 
+25/02/2025 SE COMUNICÓ EL AUTO 022 DEL 24 DE FEBRERO DE 2025 
+20/02/2025 SE PROFIRIO EL AUTO 017 Y SE NOFITICÓ EL DÍA 17/02/2025
+06/02/2025 - A LA ESPERA DECISIÓN DEL PARTIDO CAMBIO RADICAL 
+A LA ESPERA DECISIÓN DEL PARTIDO CAMBIO RADICAL </t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A LAURA ORTEGON
+28/04/2025 SE REALIZA NUEVO AUTO QUE EXHORTA EN REVISIÓN DE SHANNERY
+21/04/2025 EL REPRESENTANTE LEGAL ALLEGA PARCIALMENTE LO SOLICITADO POR AUTO 032
+07/04/2025 SE REALIZO AUTO 032 DEL 2 DE ABRIL QUE EXHORTA AL PARTIDO - SE ENVIA PARA SU DEBIDA FIRMA POR PARTE DEL PRESIDENTE EL 2 DE ABRIL DE 2025 
+27/03/2025 REALIZACIÓN DE AUTO DE INSTAR
+17/03/2025 UNA VEZ ENVIEN LA INFORMACION SE PROCEDE A INSCRIBIR LOS CANDIDATOS O A NEGAR LA INSCRIPCIÓN
+06/03/2025 SIGUE EN REVISIÓN AUTO
+27/02/2025 AUTO ENVIADO A SHAN EL 25 DE FEBRERO
+20/02/2025 ESTA EN REVISIÓN OTRO AUTO QUE DECRETA PRUEBAS SOLICITANDOLE AL PARTIDO DE LA U DOCUMENTOS PARA LA INSCRIPCIÓN DE DIRECTIVOS DEL DIRECTORIO DEPARTAMENTAL DEL VALLE DEL CAUCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORIGEN: ANDREA TOBAR: DESTINO LAURA ORTEGON </t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A LA ASESORA STEPHANI GUERRERO
+28/04/2025 A LA ESPERA DE COMUNICACIONES</t>
+  </si>
+  <si>
+    <t>ORIGEN: ANDREA TOBAR DESTINO: STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A LA ASESORA STEPHANI GUERRERO
+28/04/2025 EN ESPERA DE COMUNICACIONES PARA INICIAR AUTO DE ALEGATOS
+07/04/2025 EN ESPERA DE SU DEBIDA NOTIFICACION
+27/03/2025 SE REALIZA FORMULACIÓN DE CARGOS EN CONTRA DEL EXCANDIDATO, SE RADICO EN SALA EL 20 DE MARZO 
+14/03/2025 EN PROCESO DE REALIZACION RESOLUCION DE FORMULACION DE CARGOS AL EX GERENTE DE CAMPAÑA 
+06/03/2025 EN ESPERA DE TERMINO PARA REALIZAR AUTO DE ALEGATOS (10/03/2025)
+27/02/2025 - EN ESPERA DEL TERMINO PARA INICIAR AUTO DE ALEGATOS DE CONCLUSIÓN. 
+21/02/2025 - EN ESPERA DE QUE ALLEGUEN DESCARGOS
+13/02/2024 - EN ESPERA DE COMUNICACIONES 
+04/02/2025 A LA ESPERA DE COMUNICACIONES
+23/01/2025 EN ESPERA DE COMUNICACIÓN
+15/01/2025 PONENCIA PARA RADICAR EN SALA 
+PENDIENTE EN NOTIFICACION</t>
+  </si>
+  <si>
+    <t>ORIGEN: GÉNESIS CUELLO DESTINO: STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-008714</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMISIÓN DE RESOLUCIÓN NO. 030 DE 2025 POR MEDIO DE LA CUAL SE ORDENA CONFORMACIÓN DE UNA DIRECCIÓN DEPARTAMENTAL, Y COMITÉ EJECUTIVO DEPARTAMENTAL DEL DEPARTAMENTO DE SANTANDER DEL PARTIDO DEMÓCRATA COLOMBIANA </t>
+  </si>
+  <si>
+    <t>PEDRO ADÁN TORRES PEREZ</t>
+  </si>
+  <si>
+    <t>15/05/2025 RECIBIDO POR LA ASESORA ANYI AGURRE</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1422,6 +1381,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFF8F9FA"/>
       </patternFill>
     </fill>
   </fills>
@@ -1477,7 +1442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1538,6 +1503,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1842,241 +1816,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="17" width="66.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="216.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="5">
-        <v>46733</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="204" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46779</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="I6" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,269 +1881,322 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="B2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>285</v>
+      <c r="C2" s="9">
+        <v>45086</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>286</v>
+        <v>54</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>287</v>
+        <v>55</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>288</v>
+        <v>56</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>289</v>
+        <v>57</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="9">
+        <v>46164</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="I2" s="9">
-        <v>46535</v>
-      </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="9">
+        <v>45761</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="6">
+        <v>45791</v>
+      </c>
+      <c r="O2" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45070</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="9">
+        <v>46166</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="9">
+        <v>45735</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="9">
-        <v>46992</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>145</v>
+      <c r="N3" s="6">
+        <v>45761</v>
+      </c>
+      <c r="O3" s="6">
+        <v>45691</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>283</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>300</v>
+        <v>91</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>301</v>
+      <c r="C4" s="9">
+        <v>45684</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>302</v>
+        <v>92</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="9">
+        <v>46710</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="9">
+        <v>45722</v>
+      </c>
+      <c r="M4" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="N4" s="5">
+        <v>45792</v>
+      </c>
+      <c r="O4" s="6">
+        <v>45685</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46804</v>
-      </c>
-      <c r="J4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:17" ht="293.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45541</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" s="9">
+        <v>46636</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="9">
+        <v>45705</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="N5" s="9">
+        <v>45792</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="N4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="6" t="s">
+    </row>
+    <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45100</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="9">
+        <v>46172</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="9">
+        <v>45708</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q4" s="7" t="s">
+      <c r="N6" s="9">
+        <v>45792</v>
+      </c>
+      <c r="O6" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="9">
-        <v>45776</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="9">
-        <v>45776</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="N5" s="9">
-        <v>45776</v>
-      </c>
-      <c r="O5" s="9">
-        <v>45714</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q5" s="7" t="s">
+    <row r="7" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45791</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="9">
-        <v>45417</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="9">
-        <v>45782</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="N6" s="6">
-        <v>45783</v>
-      </c>
-      <c r="O6" s="6">
-        <v>45714</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q6" s="7" t="s">
+      <c r="G7" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="9">
+        <v>45792</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="N7" s="9">
+        <v>45792</v>
+      </c>
+      <c r="O7" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2407,7 +2204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE6D97-3CA4-4CCD-93A2-5E21B1D09E30}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -2475,43 +2272,43 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>319</v>
+        <v>273</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C2" s="13">
         <v>45779</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>320</v>
+        <v>274</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>321</v>
+        <v>275</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>322</v>
+        <v>276</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>323</v>
+        <v>277</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>324</v>
+        <v>278</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>325</v>
+        <v>279</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="13">
         <v>45779</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>325</v>
+        <v>279</v>
       </c>
       <c r="N2" s="6">
         <v>45779</v>
@@ -2520,10 +2317,10 @@
         <v>45779</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>326</v>
+        <v>280</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2532,11 +2329,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,109 +2395,109 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9">
-        <v>45086</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="9">
-        <v>46164</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="9">
-        <v>45761</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="N2" s="6">
-        <v>45791</v>
-      </c>
-      <c r="O2" s="6">
-        <v>45691</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45790</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="306" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9">
-        <v>45070</v>
+      <c r="C3" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="I3" s="9">
+        <v>45790</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="9">
-        <v>46166</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="9">
-        <v>45735</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="N3" s="6">
-        <v>45761</v>
-      </c>
-      <c r="O3" s="6">
-        <v>45691</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="Q3" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2709,342 +2506,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q6"/>
-  <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="17" width="30.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="5">
-        <v>45790</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="306" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="9">
-        <v>45790</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46172</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="408" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I5" s="5">
-        <v>46710</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="5">
-        <v>46257</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
@@ -3112,467 +2573,467 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="I2" s="5">
         <v>45298</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="9">
         <v>45701</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="9">
         <v>46174</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="I5" s="9">
         <v>46145</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="9">
         <v>46613</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="I7" s="9">
         <v>46783</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="M7" s="7" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="N7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P7" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="O7" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="Q7" s="7" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="153" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="I8" s="9">
         <v>46342</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="Q9" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="48" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>333</v>
+        <v>286</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C10" s="19">
         <v>45782</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>334</v>
+        <v>287</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>335</v>
+        <v>288</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>336</v>
+        <v>289</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" s="19">
         <v>45789</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>336</v>
+        <v>289</v>
       </c>
       <c r="N10" s="5">
         <v>45789</v>
@@ -3581,10 +3042,10 @@
         <v>45789</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3592,12 +3053,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3660,214 +3121,55 @@
     </row>
     <row r="2" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>193</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I2" s="5">
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="I3" s="9">
-        <v>46315</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="395.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46549</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="I5" s="9">
-        <v>46636</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3875,12 +3177,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q3"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3941,110 +3243,269 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="344.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="I2" s="5">
-        <v>45466</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
+      <c r="C2" s="23">
+        <v>45264</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" s="23">
+        <v>46315</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="23">
+        <v>45735</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="N2" s="9">
+        <v>45792</v>
+      </c>
+      <c r="O2" s="23">
+        <v>45691</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>238</v>
+      <c r="A3" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q3" s="7" t="s">
+      <c r="C3" s="24">
+        <v>45653</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="24">
+        <v>46549</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="24">
+        <v>45712</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="N3" s="9">
+        <v>45792</v>
+      </c>
+      <c r="O3" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="344.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45466</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>32</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="6">
+        <v>45466</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45673</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="N4" s="5">
+        <v>45755</v>
+      </c>
+      <c r="O4" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24">
+        <v>45665</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="24">
+        <v>45700</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="N5" s="5">
+        <v>45755</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45684</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="9">
+        <v>46779</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="9">
+        <v>45735</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="N6" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O6" s="6">
+        <v>45688</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4052,7 +3513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
@@ -4120,108 +3581,108 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>246</v>
+        <v>213</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>247</v>
+        <v>214</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>249</v>
+        <v>216</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>251</v>
+        <v>218</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>253</v>
+        <v>220</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>255</v>
+        <v>222</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>256</v>
+        <v>223</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="I3" s="9">
         <v>46395</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>260</v>
+        <v>227</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>252</v>
+        <v>219</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -4229,12 +3690,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4296,162 +3757,162 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>261</v>
+      <c r="A2" s="14" t="s">
+        <v>228</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="5">
+        <v>229</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43999</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="6">
         <v>44967</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>267</v>
+      <c r="J2" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45615</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="N2" s="6">
-        <v>45776</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+        <v>45791</v>
+      </c>
+      <c r="O2" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="204" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45266</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="204" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="F3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="5">
+        <v>46232</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="5">
+        <v>45693</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="N3" s="6">
+        <v>45791</v>
+      </c>
+      <c r="O3" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="9">
-        <v>46232</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="N3" s="6">
-        <v>45776</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q3" s="7" t="s">
+      <c r="C4" s="6">
+        <v>44861</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="F4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="H4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="6">
         <v>45790</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>56</v>
+      <c r="J4" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45720</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="N4" s="6">
-        <v>45776</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>32</v>
+        <v>45761</v>
+      </c>
+      <c r="O4" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -4459,7 +3920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -4527,7 +3988,7 @@
     </row>
     <row r="2" spans="1:17" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>317</v>
+        <v>271</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>18</v>
@@ -4536,34 +3997,34 @@
         <v>45700</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="I2" s="13">
         <v>46795</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="13">
         <v>45744</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>318</v>
+        <v>272</v>
       </c>
       <c r="N2" s="6">
         <v>45777</v>
@@ -4572,10 +4033,505 @@
         <v>45701</v>
       </c>
       <c r="P2" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45440</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="I2" s="5">
+        <v>46535</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="5">
+        <v>45714</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="N2" s="6">
+        <v>45775</v>
+      </c>
+      <c r="O2" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45715</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5">
+        <v>46992</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="5">
+        <v>45784</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="N3" s="6">
+        <v>45791</v>
+      </c>
+      <c r="O3" s="6">
+        <v>45715</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45709</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="9">
+        <v>46804</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="9">
+        <v>45735</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="N4" s="6">
+        <v>45761</v>
+      </c>
+      <c r="O4" s="6">
+        <v>45713</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45417</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="9">
+        <v>45786</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="N5" s="6">
+        <v>45791</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45714</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45776</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="9">
+        <v>45786</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="N6" s="9">
+        <v>45791</v>
+      </c>
+      <c r="O6" s="9">
+        <v>45714</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45758</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="5">
+        <v>45775</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="N7" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O7" s="6">
+        <v>45775</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45638</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="5">
+        <v>46733</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="5">
+        <v>45748</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="N8" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O8" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="102" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45161</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="5">
+        <v>46257</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="5">
+        <v>45370</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O9" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16 de mayo actualizacion
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FB5BE9-832C-40D8-AD92-7AC27944575D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EEEC15-6E1B-425B-9A58-593595045BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANYI AGUIRRE" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="251">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>DESPACHO</t>
-  </si>
-  <si>
-    <t>01/04/2025</t>
   </si>
   <si>
     <t>28/04/2025</t>
@@ -156,12 +153,6 @@
 26/02/2025 POR MEDIO DEL CUAL SE LE SOLICITO AL PARTIDO DE LA U SE REMITE A UNA INFORMACION IMPORTANTE PARA PROCEDER A LA INSCRIPCIÓN DE LOS DIRECTIVOS DEPARTAMENTALES DEL VALLE DEL CAUCA
 06/02/2025 AUTO No 014 POR MEDIO DE LA CUAL SE LE SOLICITAN LAS PRUEBAS A DIRECCION DE INSPECCIÓN Y VIGILANCIA
 28/01/2025 - RECIBIDO POR EL ASESOR JUAN DAVID</t>
-  </si>
-  <si>
-    <t>19/03/2025</t>
-  </si>
-  <si>
-    <t>31/01/2025</t>
   </si>
   <si>
     <t>04/03/2025</t>
@@ -305,12 +296,6 @@
 20/01/2025 - RECIBIDO</t>
   </si>
   <si>
-    <t>20/02/2025</t>
-  </si>
-  <si>
-    <t>06/12/2023</t>
-  </si>
-  <si>
     <t>OFICIO</t>
   </si>
   <si>
@@ -318,9 +303,6 @@
   </si>
   <si>
     <t>26/02/2025 RECIBIDO</t>
-  </si>
-  <si>
-    <t>26/02/2025</t>
   </si>
   <si>
     <t>CNE-E-DG-2025-001275</t>
@@ -345,13 +327,7 @@
 28/02/2025 RECIBIDO</t>
   </si>
   <si>
-    <t>22/04/2025</t>
-  </si>
-  <si>
     <t>2021-000146 - 2021-000147</t>
-  </si>
-  <si>
-    <t>07/01/2021</t>
   </si>
   <si>
     <t>SOLICITUD DE LIQUIDACION DE LA ORGANIZACIÓN POLITICA (OPCION CIUDADANA)</t>
@@ -368,23 +344,6 @@
 19/11/2024 EL AUTO 133 SE DEJA SIN DEFECTOS DESIGNACIÓN DEL LIQUIDADOR</t>
   </si>
   <si>
-    <t>10/02/2025</t>
-  </si>
-  <si>
-    <t>28/04/2025 EN ESPERA RESPUESTA FONDO NACIONAL DE FINANCIACIÓN (SE REMITIÓ OFICIO AL PARTIDO OPCIÓN CIUDADANA)
-07/04/2025 EN ESPERA RESPUESTA FONDO NACIONAL DE FINANCIACIÓN (SE REMITIÓ OFICIO AL PARTIDO OPCIÓN CIUDADANA)
-28/03/2025 EN ESPERA RESPUESTA FONDO NACIONAL DE FINANCIACIÓN (SE REMITIÓ OFICIO AL PARTIDO OPCIÓN CIUDADANA)
-18/03/2025 EN ESPERA RESPUESTA FONDO NACIONAL DE FINANCIACIÓN (SE REMITIÓ OFICIO AL PARTIDO OPCIÓN CIUDADANA)
-06/03/2025 EN ESPERA DE CUMPLIMIENTO DE TERMINOS
-21/02/2025 EN ESPERA DE CUMPLIMIENTO DE TERMINOS
-22/01/2025 EL FONDO NACIONAL DE FINANCIACIÓN DE PARTIDOS POLÍTICOS, REMITIÓ RESPUESTA ACERCA DE LO SOLICITADO A TRAVÉS DEL AUTO NO.133 DE 2025. (EN ESPERA DE INDICACIONES DEL MAGISTRADO)
-16/01/2024 SE REMITIÓ OFICIO NO. 006 DE REITERACIÓN PARA FIRMA DEL MAGISTRADO CÉSAR LORDUY
-SHANNERY INDICO REALIZAR OFICIO DE REITERACIÓN</t>
-  </si>
-  <si>
-    <t>09/01/2025</t>
-  </si>
-  <si>
     <t>JHON TRUJILLO</t>
   </si>
   <si>
@@ -392,9 +351,6 @@
   </si>
   <si>
     <t>CNE-E-DG-2022-006531</t>
-  </si>
-  <si>
-    <t>07/03/2022</t>
   </si>
   <si>
     <t>DENUNCIA POR IRREGULARIDAD POR LA FINANCIACION DE CAMPAÑA EN CONTRA DE LA SEÑORA MAYRA ALEJANDRA GAONA PINZÓN, CANDIDATO A LA CAMARA TRANSITORIA DE PAZ</t>
@@ -407,17 +363,6 @@
 20/02/2025 VIENE DERROTADO DEL DESPACHO DEL MAGISTRADO ALFONSO CAMPO</t>
   </si>
   <si>
-    <t>28/03/2025</t>
-  </si>
-  <si>
-    <t>28/04/2025 PENDIENTE DE COMUNICACIONES
-07/04/2025 PENDIENTE DE COMUNICACIONES
-28/03/2025 PENDIENTE DE COMUNICACIONES
-18/03/2025 PONENCIA RADICADA PARA DISCUSIÓN EL 20 DE MARZO DE 2025
-06/03/2025 SIGUE PENDIENTE PONENCIA EN PROYECCIÓN
-20/02/2025 PENDIENTE DE PROYECCIÓN</t>
-  </si>
-  <si>
     <t>DERROTADO DEL MAGISTRADO ALFONSO CAMPO ENCARGADO: JHON TRUJILLO</t>
   </si>
   <si>
@@ -427,23 +372,10 @@
     <t>PRESUNTA VULNERACIÓN AL ARTÍCULO 18 DE LA LEY 1475 DE 2011, UNA VEZ REVISADO INFORME DECLARACIÓN DE PATRIMONIO, INGRESOS Y GASTOS DE FUNCIONAMIENTO VIGENCIA 2022 DEL PARTIDO COLOMBIA RENACIENTE</t>
   </si>
   <si>
-    <t>28/04/2025 PROYECTANDO RESOLUCIÓN
-07/04/2025 AUN SE ESTA PROYECTANDO LA RESOLUCION
-28/03/2025 PROYECTAR RESOLUCION
-18/03/2025 ESTA EN ESPERA DE INFORME DEL CONTADOR FEISAL
-06/03/2025 EN REVISIÓN</t>
-  </si>
-  <si>
-    <t>27/02/2025</t>
-  </si>
-  <si>
     <t>ORIGEN: CAMILA REYES DESTINO: JHON TRUJILLO</t>
   </si>
   <si>
     <t>CNE-E-DG-2024-010332</t>
-  </si>
-  <si>
-    <t>03/05/2023</t>
   </si>
   <si>
     <t>RECONOMIENTO Y INSCRIPCION DEL NUEVO PRESIDENTE Y REPRESANTE LEGAL DEL PARTIDO ESPERANZA DEMÓCRATICA</t>
@@ -464,29 +396,10 @@
  28/11/2024 OFICIO N° 445 RESPUESTA MIGUEL ANGEL PEREZ GAMBOA</t>
   </si>
   <si>
-    <t>18/03/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/04/2025 EN ESPERA DE TERMINOS PARA ARCHIVO
-07/04/2025 SIGUE EN ESPERA DE NOTIFICACION PARA POSTERIOR ARCHIVO
-28/03/2025 SIGUE EN ESPERA DE NOTIFICACION PARA POSTERIOR ARCHIVO
-18/03/2025 EN ESPERA DE NOTIFICACION PARA POSTERIOR ARCHIVO
-06/03/2025 PONENCIA RESUELVE RECURSO CONTRA RESOLUCION No 00173 DE 2025 EN REVISIÓN DE SHANNERY
-ENVIADO A REVISIÓN A LAURA ORTEGON EL DÍA 20/02/2025
-13/02/2025 EN PROYECCION DE RESOLUCIÓN QUE RESUELVE RECURSOS DE  REPOSICIÓN INTERPUESTOS
-06/02/2025 - EN ESPERA DE NOTIFICACIONES Y TÉRMINO DE PARA LA PRESENTACIÓN DE  RECURSOS DE REPOSICIÓN.
-27/01/2025 EN ESPERA DE NOTIFICACIONES Y TÉRMINO DE PARA LA PRESENTACIÓN RE RECURSOS DE REPOSICIÓN.
-8/01/2025 SE RADICO PONENCIA QUE RESUELVE RECURSO DE REPOSICIÓN CONTRA LA RESOLUCIÓN QUE RECHAZO POR EXTEMPORANEO LAS SOLICITUDES DE IMPUGNACIÓN DE LOS SEÑORES JULIO CARRASCAL, TEMILDA VANEGAS
-8/01/2025 SE REMITIÓ A REVISIÓN DE LAURA ORTEGON PONENCIA QUE RESUELVE EL RECURSO DE REPOSICIÓN INTERPUESTO CONTRA LA RESOLUCIÓN QUE ACEPTO EL DESISTIMIENTO DEL SEÑOR CARLOS ENRIQUE MC'NISH </t>
-  </si>
-  <si>
     <t>ORIGEN: DORA GARCIA DESTINO: JHON TRUJILLO</t>
   </si>
   <si>
     <t>CNE-E-DG-2024-016640</t>
-  </si>
-  <si>
-    <t>14/08/2024</t>
   </si>
   <si>
     <t>SOLICITUD DE INVESTIGACIÓN POR FINANCIACIÓN DE LA CAMPAÑA AL CONCEJO DE PARATEBUENO - CUNDINAMARCA DEL CONCEJAL ELECTO, SEÑOR JULIO TORO, POR EL PARTIDO INDEPENDIENTES.</t>
@@ -507,14 +420,6 @@
     <t>24/04/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">24/04/2025 EN ESPERA DE NOTIFICACION
-07/04/2025 APLAZADA EN ESPERA RESPUESTA FONDO NACIONAL DE FINANCIACION
-28/03/2025 ESTA EN DISCUSIÓN PARA SALA EL 1 DE ABRIL
-18/03/2025 RADICADA PONENCIA QUE DA POR TERMINADO
-06/03/2025 EN PROYECCIÓN
-06/02/2025 - AUTO DE REITERACIÒN EN REVISIÓN DE SHANNERY </t>
-  </si>
-  <si>
     <t>ORIGEN: VANESSA ROSSELL - DESTINO: JHON TRUJILLO</t>
   </si>
   <si>
@@ -537,11 +442,6 @@
 19/03/2025 RECIBIDO POR EL ASESOR JHON TRUJILLO</t>
   </si>
   <si>
-    <t>22/04/2025 EN ESPERA DE NOTIFICACIONES
-07/04/2025 EN ESPERA DE TERMINOS
-28/03/2025 PONENCIA DE APERTURA VA A SER DISCUTIDA EN SALA EL 1 DE ABRIL</t>
-  </si>
-  <si>
     <t>ORIGEN: JUAN DAVID OSPINA DESTINO: JHON TRUJILLO</t>
   </si>
   <si>
@@ -570,15 +470,6 @@
 17/03/2025 EN ESPERA DE SANCIÓN</t>
   </si>
   <si>
-    <t>28/04/2025 PENDIENTE RESOLUCIÓN SI DECIDE SANCIONAR
-07/04/2025 AUN SIGUE PENDIENTE PARA RESOLUCION SI DECIDE SANCIONAR
-31/03/2025 AUN SIGUE PENDIENTE PARA RESOLUCION SI DECIDE SANCIONAR
-17/03/2025 PENDIENTE PARA RESOLUCION SI DECIDE SANCIONAR</t>
-  </si>
-  <si>
-    <t>17/03/2025</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2025-007390</t>
   </si>
   <si>
@@ -595,9 +486,6 @@
   </si>
   <si>
     <t>22/04/2025 RECIBIDO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/04/2025 EN REVISIÓN </t>
   </si>
   <si>
     <t>CNE-E-DG-2022-022511 - SANTANDER</t>
@@ -929,9 +817,6 @@
   </si>
   <si>
     <t>DIEGO FABIAN CASTILLO QUINTERO</t>
-  </si>
-  <si>
-    <t>12/05/ 2025 RECIBIDO POR EL ASESOR</t>
   </si>
   <si>
     <t>14/04/2025AUTO No 034 -TRASLADO DE ALEGATOS PUBLICIDAD
@@ -1797,7 +1682,7 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -1806,25 +1691,25 @@
         <v>45086</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="I2" s="9">
         <v>46164</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>19</v>
@@ -1833,7 +1718,7 @@
         <v>45761</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="N2" s="6">
         <v>45791</v>
@@ -1842,15 +1727,15 @@
         <v>45691</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>17</v>
@@ -1859,16 +1744,16 @@
         <v>45070</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>18</v>
@@ -1877,7 +1762,7 @@
         <v>46166</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>19</v>
@@ -1886,7 +1771,7 @@
         <v>45735</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="N3" s="6">
         <v>45761</v>
@@ -1895,15 +1780,15 @@
         <v>45691</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>17</v>
@@ -1912,25 +1797,25 @@
         <v>45684</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I4" s="9">
         <v>46710</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>19</v>
@@ -1939,7 +1824,7 @@
         <v>45722</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="N4" s="5">
         <v>45792</v>
@@ -1948,15 +1833,15 @@
         <v>45685</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="293.25" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1965,25 +1850,25 @@
         <v>45541</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="I5" s="9">
         <v>46636</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>19</v>
@@ -1992,7 +1877,7 @@
         <v>45705</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="N5" s="9">
         <v>45792</v>
@@ -2001,15 +1886,15 @@
         <v>45691</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
@@ -2018,25 +1903,25 @@
         <v>45100</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I6" s="9">
         <v>46172</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>19</v>
@@ -2045,7 +1930,7 @@
         <v>45708</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="N6" s="9">
         <v>45792</v>
@@ -2054,42 +1939,42 @@
         <v>45691</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="9">
         <v>45791</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -2098,7 +1983,7 @@
         <v>45792</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
       <c r="N7" s="9">
         <v>45792</v>
@@ -2107,10 +1992,10 @@
         <v>45691</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2186,34 +2071,34 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="13">
         <v>45779</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>19</v>
@@ -2222,7 +2107,7 @@
         <v>45779</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="N2" s="6">
         <v>45779</v>
@@ -2231,10 +2116,10 @@
         <v>45779</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2310,108 +2195,108 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="5">
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="P2" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="306" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="I3" s="9">
         <v>45790</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="P3" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2423,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView topLeftCell="J8" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:Q10"/>
+    <sheetView tabSelected="1" topLeftCell="M8" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,238 +2371,238 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="25">
+        <v>44203</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="25">
+        <v>45298</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="25">
+        <v>45698</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="N2" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O2" s="26">
+        <v>45666</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="25">
+        <v>44627</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E3" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="25">
+        <v>45701</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="25">
+        <v>45744</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="N3" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O3" s="26">
+        <v>45708</v>
+      </c>
+      <c r="P3" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q3" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="25">
+        <v>45266</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="5">
-        <v>45298</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="H4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="25">
+        <v>46174</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="L4" s="25">
+        <v>45714</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="N4" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O4" s="26">
+        <v>45715</v>
+      </c>
+      <c r="P4" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="6" t="s">
+    </row>
+    <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45049</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="I5" s="5">
+        <v>46145</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="K5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="5">
+        <v>45734</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="N5" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q5" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="9">
-        <v>45701</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46174</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I5" s="9">
-        <v>46145</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>123</v>
+      <c r="C6" s="9">
+        <v>45518</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
@@ -2726,240 +2611,240 @@
         <v>46613</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="9">
+        <v>45771</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="N6" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O6" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45688</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="5">
+        <v>46783</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="5">
+        <v>45748</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N7" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O7" s="6">
+        <v>45744</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="17">
+        <v>45246</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="17">
+        <v>46342</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="17">
+        <v>45735</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="N8" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O8" s="21">
+        <v>45733</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="17">
+        <v>45769</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="H9" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q6" s="7" t="s">
+      <c r="I9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="102" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="9">
-        <v>46783</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="K7" s="7" t="s">
+      <c r="K9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="153" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="9">
-        <v>46342</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="48" x14ac:dyDescent="0.25">
+      <c r="L9" s="17">
+        <v>45769</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="N9" s="5">
+        <v>45793</v>
+      </c>
+      <c r="O9" s="5">
+        <v>45775</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C10" s="17">
         <v>45782</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="K10" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L10" s="17">
-        <v>45789</v>
+        <v>45792</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="N10" s="5">
-        <v>45789</v>
+        <v>45792</v>
       </c>
       <c r="O10" s="5">
         <v>45789</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3035,55 +2920,55 @@
     </row>
     <row r="2" spans="1:17" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="5">
         <v>45790</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="P2" s="4" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3159,7 +3044,7 @@
     </row>
     <row r="2" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>17</v>
@@ -3168,25 +3053,25 @@
         <v>45264</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="I2" s="21">
         <v>46315</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>19</v>
@@ -3195,7 +3080,7 @@
         <v>45735</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="N2" s="9">
         <v>45792</v>
@@ -3204,15 +3089,15 @@
         <v>45691</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>17</v>
@@ -3221,25 +3106,25 @@
         <v>45653</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I3" s="22">
         <v>46549</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>19</v>
@@ -3248,7 +3133,7 @@
         <v>45712</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="N3" s="9">
         <v>45792</v>
@@ -3257,15 +3142,15 @@
         <v>45691</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="344.25" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -3274,25 +3159,25 @@
         <v>45466</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="I4" s="6">
         <v>45466</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>19</v>
@@ -3301,7 +3186,7 @@
         <v>45673</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="N4" s="5">
         <v>45755</v>
@@ -3310,15 +3195,15 @@
         <v>45691</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -3327,34 +3212,34 @@
         <v>45665</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L5" s="22">
         <v>45700</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="N5" s="5">
         <v>45755</v>
@@ -3363,15 +3248,15 @@
         <v>45691</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
@@ -3380,25 +3265,25 @@
         <v>45684</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="I6" s="9">
         <v>46779</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>19</v>
@@ -3407,7 +3292,7 @@
         <v>45735</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="N6" s="6">
         <v>45792</v>
@@ -3416,10 +3301,10 @@
         <v>45688</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3495,108 +3380,108 @@
     </row>
     <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="382.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="I3" s="9">
         <v>46395</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3672,43 +3557,43 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="C2" s="6">
         <v>43999</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I2" s="6">
         <v>44967</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L2" s="6">
         <v>45615</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="N2" s="6">
         <v>45791</v>
@@ -3717,15 +3602,15 @@
         <v>45691</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>17</v>
@@ -3734,25 +3619,25 @@
         <v>45266</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I3" s="5">
         <v>46232</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>19</v>
@@ -3761,7 +3646,7 @@
         <v>45693</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="N3" s="6">
         <v>45791</v>
@@ -3770,15 +3655,15 @@
         <v>45691</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>17</v>
@@ -3787,25 +3672,25 @@
         <v>44861</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="I4" s="6">
         <v>45790</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>19</v>
@@ -3814,7 +3699,7 @@
         <v>45720</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="N4" s="6">
         <v>45761</v>
@@ -3823,10 +3708,10 @@
         <v>45691</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3902,7 +3787,7 @@
     </row>
     <row r="2" spans="1:17" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>17</v>
@@ -3911,25 +3796,25 @@
         <v>45700</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="I2" s="13">
         <v>46795</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>19</v>
@@ -3938,7 +3823,7 @@
         <v>45744</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="N2" s="6">
         <v>45777</v>
@@ -3947,10 +3832,10 @@
         <v>45701</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3962,8 +3847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4026,7 +3911,7 @@
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>17</v>
@@ -4035,25 +3920,25 @@
         <v>44203</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I2" s="25">
         <v>45298</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="K2" s="24" t="s">
         <v>19</v>
@@ -4062,7 +3947,7 @@
         <v>45698</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="N2" s="5">
         <v>45793</v>
@@ -4071,15 +3956,15 @@
         <v>45666</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>17</v>
@@ -4088,16 +3973,16 @@
         <v>44627</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="H3" s="24" t="s">
         <v>18</v>
@@ -4106,7 +3991,7 @@
         <v>45701</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="K3" s="24" t="s">
         <v>19</v>
@@ -4115,7 +4000,7 @@
         <v>45744</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="N3" s="5">
         <v>45793</v>
@@ -4124,15 +4009,15 @@
         <v>45708</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="27" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="178.5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>17</v>
@@ -4141,16 +4026,16 @@
         <v>45266</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>18</v>
@@ -4159,7 +4044,7 @@
         <v>46174</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K4" s="24" t="s">
         <v>19</v>
@@ -4168,7 +4053,7 @@
         <v>45714</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="N4" s="5">
         <v>45793</v>
@@ -4177,15 +4062,15 @@
         <v>45715</v>
       </c>
       <c r="P4" s="27" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="11" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>17</v>
@@ -4194,34 +4079,34 @@
         <v>45049</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="I5" s="5">
         <v>46145</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L5" s="5">
         <v>45734</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="N5" s="5">
         <v>45793</v>
@@ -4230,15 +4115,15 @@
         <v>45691</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
@@ -4247,16 +4132,16 @@
         <v>45518</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>18</v>
@@ -4265,7 +4150,7 @@
         <v>46613</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>19</v>
@@ -4274,7 +4159,7 @@
         <v>45771</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="N6" s="5">
         <v>45793</v>
@@ -4283,15 +4168,15 @@
         <v>45691</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
@@ -4300,25 +4185,25 @@
         <v>45688</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I7" s="5">
         <v>46783</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>19</v>
@@ -4327,7 +4212,7 @@
         <v>45748</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="N7" s="5">
         <v>45793</v>
@@ -4336,15 +4221,15 @@
         <v>45744</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>17</v>
@@ -4353,25 +4238,25 @@
         <v>45246</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="I8" s="17">
         <v>46342</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="K8" s="19" t="s">
         <v>19</v>
@@ -4380,7 +4265,7 @@
         <v>45735</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="N8" s="5">
         <v>45793</v>
@@ -4389,42 +4274,42 @@
         <v>45733</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q8" s="16" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C9" s="17">
         <v>45769</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>19</v>
@@ -4433,7 +4318,7 @@
         <v>45769</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="N9" s="5">
         <v>45793</v>
@@ -4442,42 +4327,42 @@
         <v>45775</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C10" s="17">
         <v>45782</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="K10" s="19" t="s">
         <v>19</v>
@@ -4486,7 +4371,7 @@
         <v>45792</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="N10" s="5">
         <v>45792</v>
@@ -4495,10 +4380,10 @@
         <v>45789</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion 26 de mayo
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23000D9-5323-46B4-A274-E3CD0A9123AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A733CF-29FE-4CBB-A32B-FCF535D0151D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANYI AGUIRRE" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="333">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -998,8 +998,326 @@
 15/01/2025 SE DEBE CORRER TRASLADO</t>
   </si>
   <si>
-    <t>14/05/2025 REALIZADA AUDIENCIA PÚBLICA
-02/05/2025 ASIGNADO A LA ASESORA SHANNERY CHAPARRO</t>
+    <t>CNE-E-DG-2025-009162</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE REGISTRO DE LOGOTIPO DE LA LISTA DENOMINADA "FUERZA JOVEN" PARA EL CONSEJO DE JUVENTUDES EN EL MUNICIPIO  DE  LA APARTADA FRONTERA CORDOBA</t>
+  </si>
+  <si>
+    <t>LA APARTADA</t>
+  </si>
+  <si>
+    <t>COORDINACIÓN DE INSCRIPCIÓN DE CANDIDATOS</t>
+  </si>
+  <si>
+    <t>REGISTRO DE LOGO</t>
+  </si>
+  <si>
+    <t>RECIBIDO POR LA ASESORA ANYI AGUIRRE</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-009346</t>
+  </si>
+  <si>
+    <t>QUEJA POR POSIBLE HECHOS ANÓMALOS EN EL MUNICIPIO DE LA JAGUA DEL PILAR LA GUAJIRA DURANTE EL DESARROLLO DE LA ELECCIONES ATÍPICAS DEL 18 DE MAYO DE 2025</t>
+  </si>
+  <si>
+    <t>LA GUAJIRA</t>
+  </si>
+  <si>
+    <t>LA GAJUA DEL PILAR</t>
+  </si>
+  <si>
+    <t>FABIAN VICENTE COTES GONZALEZ</t>
+  </si>
+  <si>
+    <t>DELITO ELECTORAL</t>
+  </si>
+  <si>
+    <t>23/05/ 2025 RECIBIDO POR EL ASESOR JHON TRUJILLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO </t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-009181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SOLICITUD DE REGISTRO DE LOGOTIPO DE LA LISTA DENOMINADA "JUVENTUDES ODS" PARA EL CONSEJO DE JUVENTUDES EN EL MUNICIPIO DE VILLAVICENCIO META</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>VILLAVICENCIO</t>
+  </si>
+  <si>
+    <t>RECIBIDO POR EL ASESOR JHON TRUJILLO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-009351</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE REGISTRO DE LOGOTIPO DE LA LISTA DENOMINADA "VOCES INCLUYENTES" PARA EL CONSEJO DE JUVENTUDES EN EL MUNICIPIO DE SANTA ROSA - META</t>
+  </si>
+  <si>
+    <t>SANTA ROSA</t>
+  </si>
+  <si>
+    <t>REGISTRO LOGO</t>
+  </si>
+  <si>
+    <t>RECIBIDO POR EL ASESOR MIGUEL CALDERON</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2024-012113</t>
+  </si>
+  <si>
+    <t>ACCIÓN DE PROTECCION DE DERECHOS DE OPOSICIÓN CONTRA ALCALDIA DE ACHÍ- BOLIVAR POR POSIBLE VULNERCIÓN AL ARTICULO 16 DE LA LEY 1909 DE 2018</t>
+  </si>
+  <si>
+    <t>BOLIVAR</t>
+  </si>
+  <si>
+    <t>ACHÍ</t>
+  </si>
+  <si>
+    <t>RAMON GUSTAVO NIEBLES MERCADO</t>
+  </si>
+  <si>
+    <t>26/02/2025 AUTO CORRE TRASLADO PARA PRESENTAR ALEGATOS DE CONCLUSIÓN A LA ALCALDÍA DE ACHÍ- BOLÍVAR.
+12/12/2024 RESOLUCIÓN NO. 6620, POR MEDIO DE LA CUAL SE FORMULA CARGOS A LA ALCALDÍA DE ACHÍ BOLÍVAR 
+25/10/24 PONENCIA NO. 16077 RADICADA EN SALA POR MEDIO DE LA CUAL SE FORMULA CARGOS A LA ALCALDÍA DE ACHÍ BOLÍVAR (EN CONJUECES).
+24/07/24 RESOLUCIÓN NO. 03881 POR MEDIO DE LA CUAL SE AMPARA EL DERECHO DE OPOSICIÓN. APROBADA EN SALA DEL 24/07/24. FINALIZA TÉRMINO PARA ALLEGAR PRUEBAS DE LO ORDENADO EL 17/09.
+16/07/24 AUTO NO. 097 POR MEDIO DEL CUAL SE DECRETA UNA PRUEBA.
+30/05/24 AUTO NO. 074 POR MEDIO DEL CUAL SE AVOCÓ CONOCIMIENTO.</t>
+  </si>
+  <si>
+    <t>28/04/2025 PONENCIA RADICADA EN SALA POR MEDIO DEL CUAL SE SANCIONA A LA ALCALDIA
+03/04/2025 PONENCIA RADICADA EN SALA POR MEDIO DE LA CUAL SE SANCIONA LA ALCALDIA
+28/03/2025 PONENCIA DE SANCIÓN EN REVISIÓN DEL PRIMER FILTRO CON FECHA DEL 28
+14/03/2025 PENDIENTE PROYECTAR DECISIÓN 
+06/03/2025 EN VENCIMIENTO DETÉRMINOS PARA PRESENTAR ALEGATOS EL 13/03/2025.
+27/02/2025 VENCE TÉRMINOS PARA PRESENTAR ALEGATOS EL 13/03/2025.
+20/02/2025 SE VENCIÓ TÉRMINOS PARA ALLEGAR DESCARGOS EL 19/02/2025. PENDIENTE PROYECTAR AUTO DE ALEGATOS
+VENCE TÉRMINO PARA ALLEGAR DESCARGOS EL DÍA 19/02/2025</t>
+  </si>
+  <si>
+    <t>STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-003389</t>
+  </si>
+  <si>
+    <t>DENUNCIA CONTRA LA CAMPAÑA DEL ACTUAL ALCANDE JOHN GERMAN RAMIREZ HERNANDEZ, POR SUPUESTO APORTE DE FINANCIACIÓN</t>
+  </si>
+  <si>
+    <t>SAN MARTIN DE LOS LLANOS</t>
+  </si>
+  <si>
+    <t>CAMILO MORENO</t>
+  </si>
+  <si>
+    <t>07/05/2025 AUTO No. 043 DE 2025, POR MEDIO DEL CUAL SE DECRETA LA PRACTICA DE PRUEBAS
+04/03/2025 AUTO No 025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO Y SE DECRETAN PRUEBAS
+27/02/2025 RECIBIDO</t>
+  </si>
+  <si>
+    <t>16/05/2025 SECRETARÍAALLEGA OFICIO DE NOTIFICACIÓN DE AUTO N° 043 
+AUTO No. 043 DE 2025, POR MEDIO DEL CUAL SE DECRETA LA PRACTICA DE PRUEBAS 
+07/05/2025 AUTO No. 043 DE 2025, POR MEDIO DEL CUAL SE DECRETA LA PRACTICA DE PRUEBAS 
+28/04/2025 EN REVISIÓN DE SHANNERY AUTO DECRETA PRUEBA
+07/04/2025 EN ESPERA DE LOS TERMINOS PARA QUE SE ALLEGUEN PRUEBAS
+28/03/2025 EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS
+14/03/2025  EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS
+06/03/2025 EN TERMINO PARA QUE SE ALLEGUEN PRUEBAS</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-003216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUEJA SOBRE LA FINANCIACIÓN DE LA CAMPAÑA COMO CANDIDATO, DEL ACTUAL ALCALDE DEL MUNICIPIO DE COTA - CUNDINAMARCA, SEÑOR NESTOR ORLANDO BALSERO GARCÍA </t>
+  </si>
+  <si>
+    <t>COTA</t>
+  </si>
+  <si>
+    <t>JAIME ALCIDES RODRIGUEZ PEÑA</t>
+  </si>
+  <si>
+    <t>02/04/2025 AUTO No 030 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO Y SE ABRE INDAGACION PREMILINAR
+19/03/2025 RECIBIDO POR LA ASESORA STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>14/05/2025 AUTO REITERA EN REVISIÓN DE MIGUEL
+15/04/2025 EN ESPERA DE LOS TERMINOS PARA QUE SE ALLEGUEN PRUEBAS
+07/04/2025 PENDIENTE DE COMUNICACIONES
+28/03/2025 AUTO AVOCA EN REVISIÓN DE PRIMER FILTRO EL 20 DE MARZO DE 2025
+17/03/2025 EN PROYECCIÓN AUTO QUE AVOCA
+06/03/2025 ASESOR INDICA QUE EL EXPEDIENTE SIGUE EN REVISIÓN</t>
+  </si>
+  <si>
+    <t>ORIGEN: JUAN DAVID OSPINA DESTINO: STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-008157</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE PRÓRROGA PARA LA RECOLECCIÓN DE FIRMAS DE LA CONSULTA POPULAR DE ORIGEN CIUDADANO DENOMINADA "MUNICIPIO DE ALCALÁ EN EL ÁREA METROPOLITANA CENTRO OCCIDENTE AMCO</t>
+  </si>
+  <si>
+    <t>ALCALÁ</t>
+  </si>
+  <si>
+    <t>CARLOS ALCIDES ROJAS PEREZ</t>
+  </si>
+  <si>
+    <t>MECANISMOS DE PARTICIPACIÓN CIUDADANA</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 de 2025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 de 2025 POR MEDIO DEL CUAL SE AVOCA CONOCIMIENTO
+05/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-007754</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE RECONOCIMIENTO DE AGRUPACIÓN POLÍTICA MOVIMIENTO POLÍTICO SOCIAL COMUNAL</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>GUSTAVO GARCIA FIGUEROA Y JENNY LILIANA PULIDO VELASQUEZ</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 DE 2025 POR MEDIO DEL CUAL SE AVOCÓ CONOCIMIENTO 
+29/04/2025 RECIBIDO POR LA ASESORA STPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>09/05/2025 AUTO No. 045 DE 2025 POR MEDIO DEL CUAL SE AVOCÓ CONOCIMIENTO 
+29/04/2025 RECIBIDO POR LA ASESORA STPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-006767</t>
+  </si>
+  <si>
+    <t>REGISTRO DE NUEVOS MIEMBROS DEL CONSEJO DE CONTROL DE ETICA DEL PARTIDO COLOMBIA RENACIENTE</t>
+  </si>
+  <si>
+    <t>JHON ARLEY MURILLO BENITEZ</t>
+  </si>
+  <si>
+    <t>28/04/2025 AUTO No 037
+11/04/2025 RECIBIDO</t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A LA ASESORA STEPHANI GUERRERO
+28/04/2025 A LA ESPERA DE COMUNICACIONES</t>
+  </si>
+  <si>
+    <t>ORIGEN: ANDREA TOBAR DESTINO: STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2024-021586</t>
+  </si>
+  <si>
+    <t>PRESUNTA VULNERACIÓN DEL ART. 23 DE LA LEY 1475 DE 2011, LIMITES A LA FINANCIACIÓN PRIVADA</t>
+  </si>
+  <si>
+    <t>ARAUCA</t>
+  </si>
+  <si>
+    <t>SARAVENA</t>
+  </si>
+  <si>
+    <t>ESTEBAN FERNANDO BURBANO DUQUE</t>
+  </si>
+  <si>
+    <t>01/04/2025 RESOLUCION No 01440 APROBADA EN SALA EL 1 DE ABRIL 2025
+10/02/2025 - OFICIO N° 038 - SE REMITE COPIA DEL EXPEDIENTE AL MINISTERIO PUBLICO 
+22/01/2025   RESOLUCIÓN No. 00197 - APROBADA EN SALA 
+07/01/2025 - REMITO FORMULACIÓN DE CARGOS A REVISIÓN
+13/12/2024 RECIBIDO</t>
+  </si>
+  <si>
+    <t>15/05/2025 REASIGNADO A LA ASESORA STEPHANI GUERRERO
+28/04/2025 EN ESPERA DE COMUNICACIONES PARA INICIAR AUTO DE ALEGATOS
+07/04/2025 EN ESPERA DE SU DEBIDA NOTIFICACION
+27/03/2025 SE REALIZA FORMULACIÓN DE CARGOS EN CONTRA DEL EXCANDIDATO, SE RADICO EN SALA EL 20 DE MARZO 
+14/03/2025 EN PROCESO DE REALIZACION RESOLUCION DE FORMULACION DE CARGOS AL EX GERENTE DE CAMPAÑA 
+06/03/2025 EN ESPERA DE TERMINO PARA REALIZAR AUTO DE ALEGATOS (10/03/2025)
+27/02/2025 - EN ESPERA DEL TERMINO PARA INICIAR AUTO DE ALEGATOS DE CONCLUSIÓN. 
+21/02/2025 - EN ESPERA DE QUE ALLEGUEN DESCARGOS
+13/02/2024 - EN ESPERA DE COMUNICACIONES 
+04/02/2025 A LA ESPERA DE COMUNICACIONES
+23/01/2025 EN ESPERA DE COMUNICACIÓN
+15/01/2025 PONENCIA PARA RADICAR EN SALA 
+PENDIENTE EN NOTIFICACION</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2023-021293</t>
+  </si>
+  <si>
+    <t>PUBLICIDAD PROPAGANDA ELECTORAL</t>
+  </si>
+  <si>
+    <t>NANCY OLIVIA BURBAN</t>
+  </si>
+  <si>
+    <t>19/03/2025 RECIBIDO POR LA ASESORA GENESIS CUELLO</t>
+  </si>
+  <si>
+    <t>28/04/2024 PROYECTANDO RECURSO INTERPUESTO A LA RESOLUCIÓN SANCIÓN
+07/04/2025 EN ESTUDIO DE EXPEDIENTE
+31/03/2025 ASESOR INDICA QUE EL EXPEDIENTE ESTA EN REVISIÓN</t>
+  </si>
+  <si>
+    <t>ORIGEN: GÉNESIS CUELLO DESTINO: STEPHANI GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-009483</t>
+  </si>
+  <si>
+    <t>SOLICITUD DE REGISTRO DE LOGOTIPO DE LA LISTA DENOMINADA "PARCHADOS BCA" PARA EL CONSEJO DE JUVENTUDES EN EL MUNICIPIO DE BARRANCABERMEJA - SANTANDER</t>
+  </si>
+  <si>
+    <t>BARRANCABERMEJA</t>
+  </si>
+  <si>
+    <t>RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-009180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SOLICITUD DE REGISTRO DE LOGOTIPO DE LA LISTA DENOMINADA "JÓVENES POR UNA MEJOR CIUDAD" PARA EL CONSEJO DE JUVENTUDES EN EL MUNICIPIO DE VILLAVICENCIO META</t>
+  </si>
+  <si>
+    <t>CNE-E-DG-2025-009133</t>
+  </si>
+  <si>
+    <t>RESOLUCIÓN 02056 DE 2025: DECLARACIÓN POLÍTICA EXTEMPORÁNEA, PARA QUE ADELANTEN LAS ACTUACIONES ADMINISTRATIVAS CORRESPONDIENTES, POR PARTE DEL PARTIDO CAMBIO RADICAL FRENTE AL GOBIERNO DE SAN ONOFRE SUCRE</t>
+  </si>
+  <si>
+    <t>SUCRE</t>
+  </si>
+  <si>
+    <t>SAN ONOFRE</t>
+  </si>
+  <si>
+    <t>RESOLUCIÓN 02056 DE 2025</t>
+  </si>
+  <si>
+    <t>DECLARACION POLITICA</t>
+  </si>
+  <si>
+    <t>AUTO 050 AVOCA CONOCIMIENTO DE LA COMPULSA DE COPIAS</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1055,6 +1373,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1193,11 +1519,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1239,9 +1566,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1281,12 +1605,151 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{2AF8BEAA-C327-4F20-8D05-10D15FA1704F}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1584,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView topLeftCell="I6" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:Q7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,17 +2429,81 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:17" ht="84" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45798</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="9">
+        <v>45798</v>
+      </c>
+      <c r="M8" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="N8" s="10">
+        <v>45799</v>
+      </c>
+      <c r="O8" s="5">
+        <v>45798</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="M8">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="2">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{657348A8-837A-4B73-9F53-9C3C0790233D}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE6D97-3CA4-4CCD-93A2-5E21B1D09E30}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="I2" sqref="I2:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +2511,7 @@
     <col min="1" max="17" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>201</v>
       </c>
@@ -2062,35 +2589,70 @@
       <c r="H2" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="38" t="s">
+        <v>326</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="13">
+        <v>45798</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="K2" s="12" t="s">
+      <c r="R2" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="S2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="13">
-        <v>45791</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="N2" s="6">
-        <v>45791</v>
-      </c>
-      <c r="O2" s="13">
-        <v>45779</v>
-      </c>
-      <c r="P2" s="12" t="s">
+      <c r="T2" s="13">
+        <v>45799</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="V2" s="13">
+        <v>45799</v>
+      </c>
+      <c r="W2" s="6">
+        <v>45803</v>
+      </c>
+      <c r="X2" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="Y2" s="12" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="U2">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{F2C53C15-E38C-4F55-A9E2-303141146E85}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2274,10 +2836,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="M8" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,40 +2901,40 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="24">
         <v>44203</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="24">
         <v>45298</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="24">
         <v>45698</v>
       </c>
       <c r="M2" s="14" t="s">
@@ -2381,51 +2943,51 @@
       <c r="N2" s="5">
         <v>45793</v>
       </c>
-      <c r="O2" s="26">
+      <c r="O2" s="25">
         <v>45666</v>
       </c>
-      <c r="P2" s="27" t="s">
+      <c r="P2" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="26" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="24">
         <v>44627</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="24">
         <v>45701</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="24">
         <v>45744</v>
       </c>
       <c r="M3" s="14" t="s">
@@ -2434,51 +2996,51 @@
       <c r="N3" s="5">
         <v>45793</v>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="25">
         <v>45708</v>
       </c>
-      <c r="P3" s="27" t="s">
+      <c r="P3" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="Q3" s="26" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>45266</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="24">
         <v>46174</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="24">
         <v>45714</v>
       </c>
       <c r="M4" s="14" t="s">
@@ -2487,13 +3049,13 @@
       <c r="N4" s="5">
         <v>45793</v>
       </c>
-      <c r="O4" s="26">
+      <c r="O4" s="25">
         <v>45715</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="26" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2543,10 +3105,10 @@
       <c r="O5" s="6">
         <v>45691</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="Q5" s="27" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2649,104 +3211,104 @@
       <c r="O7" s="6">
         <v>45744</v>
       </c>
-      <c r="P7" s="28" t="s">
+      <c r="P7" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="Q7" s="28" t="s">
+      <c r="Q7" s="27" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>45246</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <v>46342</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>45735</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="15" t="s">
         <v>238</v>
       </c>
       <c r="N8" s="5">
         <v>45793</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="20">
         <v>45733</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Q8" s="16" t="s">
+      <c r="Q8" s="15" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>45769</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="16">
         <v>45769</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="15" t="s">
         <v>239</v>
       </c>
       <c r="N9" s="5">
@@ -2755,51 +3317,51 @@
       <c r="O9" s="5">
         <v>45775</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Q9" s="16" t="s">
+      <c r="Q9" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>45782</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>45792</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="15" t="s">
         <v>240</v>
       </c>
       <c r="N10" s="5">
@@ -2808,14 +3370,140 @@
       <c r="O10" s="5">
         <v>45789</v>
       </c>
-      <c r="P10" s="16" t="s">
+      <c r="P10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="Q10" s="16" t="s">
+      <c r="Q10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="1:17" ht="72" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="16">
+        <v>45800</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="16">
+        <v>45800</v>
+      </c>
+      <c r="M11" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="N11" s="32">
+        <v>45803</v>
+      </c>
+      <c r="O11" s="16">
+        <v>45803</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="84" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="16">
+        <v>45798</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="16">
+        <v>45798</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="N12" s="32">
+        <v>45798</v>
+      </c>
+      <c r="O12" s="5">
+        <v>45798</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="M11">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="4">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="2">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A11" r:id="rId1" xr:uid="{AF103C97-F03C-4495-BDE8-87273BCE9ED5}"/>
+    <hyperlink ref="A12" r:id="rId2" xr:uid="{4F2EBC93-F0E9-40ED-852D-754C9B25DE0E}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3011,55 +3699,55 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>45264</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="20">
         <v>46315</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="21">
+      <c r="L2" s="20">
         <v>45735</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>223</v>
       </c>
       <c r="N2" s="9">
         <v>45792</v>
       </c>
-      <c r="O2" s="21">
+      <c r="O2" s="20">
         <v>45691</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="19" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3070,7 +3758,7 @@
       <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>45653</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -3088,7 +3776,7 @@
       <c r="H3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="21">
         <v>46549</v>
       </c>
       <c r="J3" s="8" t="s">
@@ -3097,7 +3785,7 @@
       <c r="K3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="21">
         <v>45712</v>
       </c>
       <c r="M3" s="8" t="s">
@@ -3112,7 +3800,7 @@
       <c r="P3" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="Q3" s="19" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3218,7 +3906,7 @@
       <c r="P5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="19" t="s">
         <v>227</v>
       </c>
     </row>
@@ -3229,10 +3917,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:Q3"/>
+      <selection activeCell="A2" sqref="A2:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,7 +4087,71 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:17" ht="72" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45800</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45800</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="O4" s="6">
+        <v>45803</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="M4">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{316F63DD-6A47-431A-8C65-B8E2F411C9AA}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3760,10 +4512,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3824,484 +4576,557 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25">
-        <v>44203</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="5">
+        <v>45440</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I2" s="5">
+        <v>46535</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="5">
+        <v>45714</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="N2" s="6">
+        <v>45775</v>
+      </c>
+      <c r="O2" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="280.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45715</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="5">
+        <v>46992</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="5">
+        <v>45784</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="N3" s="6">
+        <v>45793</v>
+      </c>
+      <c r="O3" s="6">
+        <v>45715</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45709</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="9">
+        <v>46804</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="9">
+        <v>45735</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="N4" s="6">
+        <v>45761</v>
+      </c>
+      <c r="O4" s="6">
+        <v>45713</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45417</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="J5" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="9">
+        <v>45786</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="N5" s="6">
+        <v>45791</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45714</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45776</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="25">
-        <v>45298</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="25">
-        <v>45698</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="N2" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O2" s="26">
-        <v>45666</v>
-      </c>
-      <c r="P2" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q2" s="27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="165.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="25">
-        <v>44627</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="25">
-        <v>45701</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="25">
-        <v>45744</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="N3" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O3" s="26">
-        <v>45708</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="25">
-        <v>45266</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="25">
-        <v>46174</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="25">
-        <v>45714</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="N4" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O4" s="26">
-        <v>45715</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5">
-        <v>45049</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" s="5">
-        <v>46145</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="5">
-        <v>45734</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="N5" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O5" s="6">
-        <v>45691</v>
-      </c>
-      <c r="P5" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="204" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9">
-        <v>45518</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="9">
-        <v>46613</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>107</v>
+        <v>299</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="L6" s="9">
-        <v>45771</v>
+        <v>45786</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="N6" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O6" s="6">
+        <v>300</v>
+      </c>
+      <c r="N6" s="9">
+        <v>45791</v>
+      </c>
+      <c r="O6" s="9">
+        <v>45714</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45758</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="5">
+        <v>45775</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="N7" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O7" s="6">
+        <v>45775</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45638</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="5">
+        <v>46733</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="5">
+        <v>45748</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="N8" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O8" s="6">
         <v>45691</v>
       </c>
-      <c r="P6" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="P8" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="102" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5">
-        <v>45688</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="5">
-        <v>46783</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="4" t="s">
+      <c r="C9" s="5">
+        <v>45161</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="5">
+        <v>46257</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="5">
-        <v>45748</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="N7" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O7" s="6">
-        <v>45744</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q7" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="17">
-        <v>45246</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="I8" s="17">
-        <v>46342</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" s="19" t="s">
+      <c r="L9" s="5">
+        <v>45370</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="N9" s="6">
+        <v>45792</v>
+      </c>
+      <c r="O9" s="6">
+        <v>45691</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="72" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45803</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="17">
-        <v>45735</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="N8" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O8" s="21">
-        <v>45733</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="17">
-        <v>45769</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="L10" s="9">
+        <v>45803</v>
+      </c>
+      <c r="M10" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="N10" s="10">
+        <v>45803</v>
+      </c>
+      <c r="O10" s="9">
+        <v>45803</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="96" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45798</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="K9" s="19" t="s">
+      <c r="J11" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="17">
-        <v>45769</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="N9" s="5">
-        <v>45793</v>
-      </c>
-      <c r="O9" s="5">
-        <v>45775</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="17">
-        <v>45782</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="17">
-        <v>45792</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="N10" s="5">
-        <v>45792</v>
-      </c>
-      <c r="O10" s="5">
-        <v>45789</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>25</v>
+      <c r="L11" s="9">
+        <v>45798</v>
+      </c>
+      <c r="M11" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="N11" s="10">
+        <v>45798</v>
+      </c>
+      <c r="O11" s="9">
+        <v>45798</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="M10">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{12317B88-EC32-469A-BC9F-9918DCCA964C}"/>
+    <hyperlink ref="A11" r:id="rId2" xr:uid="{C19A4EFE-C67B-4D90-A2B3-39260CA6EDB6}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion 26 de mayo-2
</commit_message>
<xml_diff>
--- a/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
+++ b/HSA VISTA GENERAL H.M ALVARO ECHEVERRY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerardo.forero\Desktop\HSA-VISTA-GENERAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A733CF-29FE-4CBB-A32B-FCF535D0151D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1FB7D7-A1F5-4977-A1FE-19E7D7F9DB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANYI AGUIRRE" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="329">
   <si>
     <t>EXPEDIENTE</t>
   </si>
@@ -737,24 +737,6 @@
 21/02/2025 ASESOR INDICA QUE NO HAY NUEVOS ACTOS ADMINISTRATIVOS</t>
   </si>
   <si>
-    <t>CNE-E-DG-2025-008134</t>
-  </si>
-  <si>
-    <t>SOLICITUD DE REVOCATORIA DE MANDATO DEL ACTUAL ALCALDE DEL MUNICIPIO DE HONDA TOLIMA, SEÑOR JUAN ENRIQUE RONDON GARCIA</t>
-  </si>
-  <si>
-    <t>TOLIMA</t>
-  </si>
-  <si>
-    <t>HONDA</t>
-  </si>
-  <si>
-    <t>CARLOS HUGO MESA MAYNE</t>
-  </si>
-  <si>
-    <t>REVOCATORIA DE MANDATO</t>
-  </si>
-  <si>
     <t>SHANNERY CHAPARRO</t>
   </si>
   <si>
@@ -1289,9 +1271,6 @@
     <t>BARRANCABERMEJA</t>
   </si>
   <si>
-    <t>RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
-  </si>
-  <si>
     <t>CNE-E-DG-2025-009180</t>
   </si>
   <si>
@@ -1317,7 +1296,16 @@
     <t>DECLARACION POLITICA</t>
   </si>
   <si>
-    <t>AUTO 050 AVOCA CONOCIMIENTO DE LA COMPULSA DE COPIAS</t>
+    <t>22/05/2025 AUTO 050 AVOCA CONOCIMIENTO DE LA COMPULSA DE COPIAS</t>
+  </si>
+  <si>
+    <t>21/05/ 2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>26/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
+  </si>
+  <si>
+    <t>21/05/2025 RECIBIDO POR LA ASESORA STEPHANIE GUERRERO</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1512,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1611,9 +1599,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1638,10 +1623,25 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1650,21 +1650,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{2AF8BEAA-C327-4F20-8D05-10D15FA1704F}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -2049,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="H6" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2126,7 @@
         <v>46164</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>19</v>
@@ -2149,7 +2135,7 @@
         <v>45761</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="N2" s="6">
         <v>45791</v>
@@ -2202,7 +2188,7 @@
         <v>45735</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="N3" s="6">
         <v>45761</v>
@@ -2255,7 +2241,7 @@
         <v>45722</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="N4" s="5">
         <v>45792</v>
@@ -2267,7 +2253,7 @@
         <v>39</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="293.25" x14ac:dyDescent="0.25">
@@ -2308,7 +2294,7 @@
         <v>45705</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="N5" s="9">
         <v>45792</v>
@@ -2320,7 +2306,7 @@
         <v>39</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -2361,7 +2347,7 @@
         <v>45708</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="N6" s="9">
         <v>45792</v>
@@ -2373,12 +2359,12 @@
         <v>39</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>28</v>
@@ -2387,7 +2373,7 @@
         <v>45791</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>133</v>
@@ -2396,7 +2382,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>30</v>
@@ -2405,7 +2391,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -2414,7 +2400,7 @@
         <v>45792</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="N7" s="9">
         <v>45792</v>
@@ -2431,7 +2417,7 @@
     </row>
     <row r="8" spans="1:17" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>28</v>
@@ -2440,25 +2426,25 @@
         <v>45798</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>19</v>
@@ -2466,8 +2452,8 @@
       <c r="L8" s="9">
         <v>45798</v>
       </c>
-      <c r="M8" s="30" t="s">
-        <v>248</v>
+      <c r="M8" s="44" t="s">
+        <v>242</v>
       </c>
       <c r="N8" s="10">
         <v>45799</v>
@@ -2484,10 +2470,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2502,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE6D97-3CA4-4CCD-93A2-5E21B1D09E30}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:Y2"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,84 +2551,76 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>201</v>
+      <c r="A2" s="37" t="s">
+        <v>319</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="13">
-        <v>45779</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>202</v>
+        <v>45798</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>320</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>203</v>
+        <v>321</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>204</v>
+        <v>322</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>326</v>
+        <v>323</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="13">
-        <v>45798</v>
-      </c>
-      <c r="L2" s="39" t="s">
-        <v>327</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="S2" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="13">
+      <c r="L2" s="13">
         <v>45799</v>
       </c>
-      <c r="U2" s="30" t="s">
-        <v>332</v>
-      </c>
-      <c r="V2" s="13">
+      <c r="M2" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="N2" s="13">
         <v>45799</v>
       </c>
-      <c r="W2" s="6">
+      <c r="O2" s="6">
         <v>45803</v>
       </c>
-      <c r="X2" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y2" s="12" t="s">
+      <c r="P2" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q2" s="12" t="s">
         <v>22</v>
       </c>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="39"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="U2">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>60</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>"m2&gt;60"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
@@ -2651,7 +2629,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{F2C53C15-E38C-4F55-A9E2-303141146E85}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DAD734E0-D319-4AF5-9A7C-2828F118D8B4}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2838,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q12"/>
+    <sheetView tabSelected="1" topLeftCell="H8" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +2916,7 @@
         <v>45698</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="N2" s="5">
         <v>45793</v>
@@ -2991,7 +2969,7 @@
         <v>45744</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="N3" s="5">
         <v>45793</v>
@@ -3044,7 +3022,7 @@
         <v>45714</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="N4" s="5">
         <v>45793</v>
@@ -3097,7 +3075,7 @@
         <v>45734</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="N5" s="5">
         <v>45793</v>
@@ -3150,7 +3128,7 @@
         <v>45771</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="N6" s="5">
         <v>45793</v>
@@ -3203,7 +3181,7 @@
         <v>45748</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="N7" s="5">
         <v>45793</v>
@@ -3256,7 +3234,7 @@
         <v>45735</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="N8" s="5">
         <v>45793</v>
@@ -3309,7 +3287,7 @@
         <v>45769</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="N9" s="5">
         <v>45793</v>
@@ -3326,7 +3304,7 @@
     </row>
     <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>126</v>
@@ -3335,7 +3313,7 @@
         <v>45782</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>25</v>
@@ -3344,7 +3322,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>198</v>
@@ -3353,7 +3331,7 @@
         <v>25</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="K10" s="18" t="s">
         <v>19</v>
@@ -3362,7 +3340,7 @@
         <v>45792</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="N10" s="5">
         <v>45792</v>
@@ -3378,8 +3356,8 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="72" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>249</v>
+      <c r="A11" s="30" t="s">
+        <v>243</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>126</v>
@@ -3388,25 +3366,25 @@
         <v>45800</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I11" s="16" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>19</v>
@@ -3414,10 +3392,10 @@
       <c r="L11" s="16">
         <v>45800</v>
       </c>
-      <c r="M11" s="30" t="s">
-        <v>255</v>
-      </c>
-      <c r="N11" s="32">
+      <c r="M11" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="N11" s="31">
         <v>45803</v>
       </c>
       <c r="O11" s="16">
@@ -3427,12 +3405,12 @@
         <v>87</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="84" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>257</v>
+      <c r="A12" s="30" t="s">
+        <v>251</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>126</v>
@@ -3441,25 +3419,25 @@
         <v>45798</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K12" s="18" t="s">
         <v>19</v>
@@ -3467,10 +3445,10 @@
       <c r="L12" s="16">
         <v>45798</v>
       </c>
-      <c r="M12" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="N12" s="32">
+      <c r="M12" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="N12" s="31">
         <v>45798</v>
       </c>
       <c r="O12" s="5">
@@ -3480,19 +3458,11 @@
         <v>87</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>"m2&gt;60"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M12">
+  <conditionalFormatting sqref="M11:M12">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
@@ -3736,7 +3706,7 @@
         <v>45735</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="N2" s="9">
         <v>45792</v>
@@ -3748,7 +3718,7 @@
         <v>163</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
@@ -3789,7 +3759,7 @@
         <v>45712</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="N3" s="9">
         <v>45792</v>
@@ -3801,7 +3771,7 @@
         <v>163</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
@@ -3833,7 +3803,7 @@
         <v>45466</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>19</v>
@@ -3842,7 +3812,7 @@
         <v>45748</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="N4" s="5">
         <v>45783</v>
@@ -3895,7 +3865,7 @@
         <v>45735</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="N5" s="6">
         <v>45792</v>
@@ -3907,7 +3877,7 @@
         <v>163</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3919,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q4"/>
+    <sheetView topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,8 +4058,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="72" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>262</v>
+      <c r="A4" s="32" t="s">
+        <v>256</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>28</v>
@@ -4097,26 +4067,26 @@
       <c r="C4" s="6">
         <v>45800</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>263</v>
+      <c r="D4" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="E4" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>265</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>19</v>
@@ -4124,11 +4094,11 @@
       <c r="L4" s="6">
         <v>45800</v>
       </c>
-      <c r="M4" s="30" t="s">
-        <v>266</v>
+      <c r="M4" s="44" t="s">
+        <v>260</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="O4" s="6">
         <v>45803</v>
@@ -4260,7 +4230,7 @@
         <v>45615</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="N2" s="6">
         <v>45791</v>
@@ -4313,7 +4283,7 @@
         <v>45693</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N3" s="6">
         <v>45791</v>
@@ -4366,7 +4336,7 @@
         <v>45720</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="N4" s="6">
         <v>45761</v>
@@ -4514,8 +4484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q11"/>
+    <sheetView topLeftCell="I8" workbookViewId="0">
+      <selection activeCell="M11" sqref="M10:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4578,7 +4548,7 @@
     </row>
     <row r="2" spans="1:17" ht="369.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>17</v>
@@ -4587,16 +4557,16 @@
         <v>45440</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>198</v>
@@ -4605,7 +4575,7 @@
         <v>46535</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>19</v>
@@ -4614,7 +4584,7 @@
         <v>45714</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="N2" s="6">
         <v>45775</v>
@@ -4623,7 +4593,7 @@
         <v>45691</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>22</v>
@@ -4631,7 +4601,7 @@
     </row>
     <row r="3" spans="1:17" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>17</v>
@@ -4640,16 +4610,16 @@
         <v>45715</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>18</v>
@@ -4658,7 +4628,7 @@
         <v>46992</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>19</v>
@@ -4667,7 +4637,7 @@
         <v>45784</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="N3" s="6">
         <v>45793</v>
@@ -4676,7 +4646,7 @@
         <v>45715</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>22</v>
@@ -4684,7 +4654,7 @@
     </row>
     <row r="4" spans="1:17" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>17</v>
@@ -4693,16 +4663,16 @@
         <v>45709</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>105</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>18</v>
@@ -4711,7 +4681,7 @@
         <v>46804</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>19</v>
@@ -4720,7 +4690,7 @@
         <v>45735</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="N4" s="6">
         <v>45761</v>
@@ -4729,15 +4699,15 @@
         <v>45713</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="11" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>28</v>
@@ -4746,25 +4716,25 @@
         <v>45417</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>291</v>
+        <v>284</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>285</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>19</v>
@@ -4773,7 +4743,7 @@
         <v>45786</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="N5" s="6">
         <v>45791</v>
@@ -4782,7 +4752,7 @@
         <v>45714</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q5" s="7" t="s">
         <v>22</v>
@@ -4790,7 +4760,7 @@
     </row>
     <row r="6" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>28</v>
@@ -4799,16 +4769,16 @@
         <v>45776</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>298</v>
+        <v>291</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>292</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>129</v>
@@ -4817,7 +4787,7 @@
         <v>25</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>19</v>
@@ -4826,7 +4796,7 @@
         <v>45786</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="N6" s="9">
         <v>45791</v>
@@ -4835,7 +4805,7 @@
         <v>45714</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>22</v>
@@ -4843,7 +4813,7 @@
     </row>
     <row r="7" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>28</v>
@@ -4852,7 +4822,7 @@
         <v>45758</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>24</v>
@@ -4861,7 +4831,7 @@
         <v>25</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>30</v>
@@ -4870,7 +4840,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>19</v>
@@ -4879,7 +4849,7 @@
         <v>45775</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="N7" s="6">
         <v>45792</v>
@@ -4888,15 +4858,15 @@
         <v>45775</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
@@ -4905,16 +4875,16 @@
         <v>45638</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>18</v>
@@ -4923,7 +4893,7 @@
         <v>46733</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>19</v>
@@ -4932,7 +4902,7 @@
         <v>45748</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="N8" s="6">
         <v>45792</v>
@@ -4941,15 +4911,15 @@
         <v>45691</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="102" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
@@ -4958,7 +4928,7 @@
         <v>45161</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>25</v>
@@ -4967,7 +4937,7 @@
         <v>25</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>45</v>
@@ -4976,7 +4946,7 @@
         <v>46257</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>19</v>
@@ -4985,7 +4955,7 @@
         <v>45370</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="N9" s="6">
         <v>45792</v>
@@ -4994,15 +4964,15 @@
         <v>45691</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>28</v>
@@ -5011,25 +4981,25 @@
         <v>45803</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>133</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>246</v>
+        <v>316</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>240</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>19</v>
@@ -5037,8 +5007,8 @@
       <c r="L10" s="9">
         <v>45803</v>
       </c>
-      <c r="M10" s="30" t="s">
-        <v>323</v>
+      <c r="M10" s="44" t="s">
+        <v>327</v>
       </c>
       <c r="N10" s="10">
         <v>45803</v>
@@ -5047,7 +5017,7 @@
         <v>45803</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>22</v>
@@ -5055,7 +5025,7 @@
     </row>
     <row r="11" spans="1:17" ht="96" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>28</v>
@@ -5064,25 +5034,25 @@
         <v>45798</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>246</v>
+        <v>254</v>
+      </c>
+      <c r="G11" s="36" t="s">
+        <v>240</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -5090,8 +5060,8 @@
       <c r="L11" s="9">
         <v>45798</v>
       </c>
-      <c r="M11" s="30" t="s">
-        <v>323</v>
+      <c r="M11" s="44" t="s">
+        <v>326</v>
       </c>
       <c r="N11" s="10">
         <v>45798</v>
@@ -5100,26 +5070,18 @@
         <v>45798</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="M10:M11">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>"m2&gt;60"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
-      <formula>60</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>"m2&gt;60"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>